<commit_message>
Edit `task-2` in `decision-support`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/decision-support/task-2/task-2.xlsx
+++ b/3-course-6-semester/decision-support/task-2/task-2.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronn\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\egor\github\university\3-course-6-semester\decision-support\task-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E877544-69CA-4B7C-99C9-4C92738901A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91462E76-BE17-4E9B-B372-FBBB535BD377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{737F3F3F-B8D1-487C-8F75-3BB915F47FFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{737F3F3F-B8D1-487C-8F75-3BB915F47FFB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Данные" sheetId="1" r:id="rId1"/>
-    <sheet name="Критерии" sheetId="2" r:id="rId2"/>
-    <sheet name="Тесты" sheetId="3" r:id="rId3"/>
+    <sheet name="(Criteria) Данные" sheetId="1" r:id="rId1"/>
+    <sheet name="(Criteria) Критерии" sheetId="2" r:id="rId2"/>
+    <sheet name="(Criteria) Тесты" sheetId="3" r:id="rId3"/>
+    <sheet name="(Pareto) Данные" sheetId="4" r:id="rId4"/>
+    <sheet name="(Pareto) Матрица" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="57">
   <si>
     <t>ВТБ</t>
   </si>
@@ -202,13 +204,19 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +241,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -272,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -508,11 +524,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -568,23 +644,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -600,6 +667,51 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -940,7 +1052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A4A19C-CE63-4B26-AAA3-ADCE19EB590C}">
   <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
@@ -950,60 +1062,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="2:14" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="33"/>
+      <c r="N3" s="30"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="33"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
@@ -1031,14 +1143,14 @@
       <c r="L4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="33"/>
+      <c r="N4" s="30"/>
     </row>
     <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="33"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="3">
         <v>11.5</v>
       </c>
@@ -1066,14 +1178,14 @@
       <c r="L5" s="3">
         <v>25</v>
       </c>
-      <c r="M5" s="27">
-        <v>1</v>
-      </c>
-      <c r="N5" s="33"/>
+      <c r="M5" s="24">
+        <v>1</v>
+      </c>
+      <c r="N5" s="30"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
-      <c r="C6" s="28" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2">
@@ -1103,14 +1215,14 @@
       <c r="L6" s="2">
         <v>50</v>
       </c>
-      <c r="M6" s="29">
-        <v>1</v>
-      </c>
-      <c r="N6" s="33"/>
+      <c r="M6" s="26">
+        <v>1</v>
+      </c>
+      <c r="N6" s="30"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="33"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="2">
@@ -1140,14 +1252,14 @@
       <c r="L7" s="2">
         <v>25</v>
       </c>
-      <c r="M7" s="29">
-        <v>1</v>
-      </c>
-      <c r="N7" s="33"/>
+      <c r="M7" s="26">
+        <v>1</v>
+      </c>
+      <c r="N7" s="30"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
-      <c r="C8" s="28" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="25" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="2">
@@ -1177,14 +1289,14 @@
       <c r="L8" s="2">
         <v>25</v>
       </c>
-      <c r="M8" s="29">
-        <v>1</v>
-      </c>
-      <c r="N8" s="33"/>
+      <c r="M8" s="26">
+        <v>1</v>
+      </c>
+      <c r="N8" s="30"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="33"/>
-      <c r="C9" s="28" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="25" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="2">
@@ -1214,14 +1326,14 @@
       <c r="L9" s="2">
         <v>25</v>
       </c>
-      <c r="M9" s="29">
-        <v>1</v>
-      </c>
-      <c r="N9" s="33"/>
+      <c r="M9" s="26">
+        <v>1</v>
+      </c>
+      <c r="N9" s="30"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
-      <c r="C10" s="28" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="25" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="2">
@@ -1251,14 +1363,14 @@
       <c r="L10" s="2">
         <v>30</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10" s="26">
         <v>0.5</v>
       </c>
-      <c r="N10" s="33"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="33"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="2">
@@ -1288,14 +1400,14 @@
       <c r="L11" s="2">
         <v>30</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="26">
         <v>2</v>
       </c>
-      <c r="N11" s="33"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="33"/>
-      <c r="C12" s="28" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2">
@@ -1325,14 +1437,14 @@
       <c r="L12" s="2">
         <v>25</v>
       </c>
-      <c r="M12" s="29">
-        <v>1</v>
-      </c>
-      <c r="N12" s="33"/>
+      <c r="M12" s="26">
+        <v>1</v>
+      </c>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
-      <c r="C13" s="28" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="25" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="2">
@@ -1362,14 +1474,14 @@
       <c r="L13" s="2">
         <v>25</v>
       </c>
-      <c r="M13" s="29">
+      <c r="M13" s="26">
         <v>2</v>
       </c>
-      <c r="N13" s="33"/>
+      <c r="N13" s="30"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="33"/>
-      <c r="C14" s="28" t="s">
+      <c r="B14" s="30"/>
+      <c r="C14" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="2">
@@ -1399,14 +1511,14 @@
       <c r="L14" s="2">
         <v>25</v>
       </c>
-      <c r="M14" s="29">
-        <v>1</v>
-      </c>
-      <c r="N14" s="33"/>
+      <c r="M14" s="26">
+        <v>1</v>
+      </c>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="33"/>
-      <c r="C15" s="28" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="2">
@@ -1436,14 +1548,14 @@
       <c r="L15" s="2">
         <v>25</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="26">
         <v>0.25</v>
       </c>
-      <c r="N15" s="33"/>
+      <c r="N15" s="30"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="33"/>
-      <c r="C16" s="28" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="25" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="2">
@@ -1473,14 +1585,14 @@
       <c r="L16" s="2">
         <v>30</v>
       </c>
-      <c r="M16" s="29">
+      <c r="M16" s="26">
         <v>2</v>
       </c>
-      <c r="N16" s="33"/>
+      <c r="N16" s="30"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="33"/>
-      <c r="C17" s="28" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="25" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="2">
@@ -1510,14 +1622,14 @@
       <c r="L17" s="2">
         <v>20</v>
       </c>
-      <c r="M17" s="29">
+      <c r="M17" s="26">
         <v>2</v>
       </c>
-      <c r="N17" s="33"/>
+      <c r="N17" s="30"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="33"/>
-      <c r="C18" s="28" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="25" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="2">
@@ -1547,14 +1659,14 @@
       <c r="L18" s="2">
         <v>25</v>
       </c>
-      <c r="M18" s="29">
-        <v>1</v>
-      </c>
-      <c r="N18" s="33"/>
+      <c r="M18" s="26">
+        <v>1</v>
+      </c>
+      <c r="N18" s="30"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="33"/>
-      <c r="C19" s="28" t="s">
+      <c r="B19" s="30"/>
+      <c r="C19" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="2">
@@ -1584,62 +1696,62 @@
       <c r="L19" s="2">
         <v>25</v>
       </c>
-      <c r="M19" s="29">
+      <c r="M19" s="26">
         <v>0.5</v>
       </c>
-      <c r="N19" s="33"/>
+      <c r="N19" s="30"/>
     </row>
     <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="33"/>
-      <c r="C20" s="30" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="28">
         <v>10.5</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="28">
         <v>25</v>
       </c>
-      <c r="F20" s="31">
+      <c r="F20" s="28">
         <v>3</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="28">
         <v>5</v>
       </c>
-      <c r="H20" s="31">
+      <c r="H20" s="28">
         <v>7.5</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I20" s="28">
         <v>9.625</v>
       </c>
-      <c r="J20" s="31">
+      <c r="J20" s="28">
         <v>0.5</v>
       </c>
-      <c r="K20" s="31">
+      <c r="K20" s="28">
         <v>60</v>
       </c>
-      <c r="L20" s="31">
+      <c r="L20" s="28">
         <v>25</v>
       </c>
-      <c r="M20" s="32">
+      <c r="M20" s="29">
         <v>1.5</v>
       </c>
-      <c r="N20" s="33"/>
+      <c r="N20" s="30"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1658,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49646155-A122-40EE-AA60-7F19038B680C}">
   <dimension ref="B2:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -1668,63 +1780,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="2:18" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="33"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="R3" s="5"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="33"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
@@ -1752,18 +1864,18 @@
       <c r="L4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="33"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="33"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="3">
         <v>11.5</v>
       </c>
@@ -1791,784 +1903,784 @@
       <c r="L5" s="3">
         <v>25</v>
       </c>
-      <c r="M5" s="27">
-        <v>1</v>
-      </c>
-      <c r="N5" s="33"/>
+      <c r="M5" s="24">
+        <v>1</v>
+      </c>
+      <c r="N5" s="30"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="33">
-        <v>1</v>
-      </c>
-      <c r="C6" s="28" t="s">
+      <c r="B6" s="30">
+        <v>1</v>
+      </c>
+      <c r="C6" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <f>INT(Данные!D6&lt;=Данные!D5)</f>
+        <f>INT('(Criteria) Данные'!D6&lt;='(Criteria) Данные'!D5)</f>
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <f>INT(Данные!E6&lt;=Данные!E5)</f>
+        <f>INT('(Criteria) Данные'!E6&lt;='(Criteria) Данные'!E5)</f>
         <v>1</v>
       </c>
       <c r="F6" s="2">
-        <f>INT(Данные!F6&lt;=Данные!F5)</f>
+        <f>INT('(Criteria) Данные'!F6&lt;='(Criteria) Данные'!F5)</f>
         <v>1</v>
       </c>
       <c r="G6" s="2">
-        <f>INT(Данные!G6&lt;=Данные!G5)</f>
+        <f>INT('(Criteria) Данные'!G6&lt;='(Criteria) Данные'!G5)</f>
         <v>0</v>
       </c>
       <c r="H6" s="2">
-        <f>INT(Данные!H6&lt;=Данные!H5)</f>
+        <f>INT('(Criteria) Данные'!H6&lt;='(Criteria) Данные'!H5)</f>
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f>INT(Данные!I6&lt;=Данные!I5)</f>
+        <f>INT('(Criteria) Данные'!I6&lt;='(Criteria) Данные'!I5)</f>
         <v>0</v>
       </c>
       <c r="J6" s="2">
-        <f>INT(Данные!J6&lt;=Данные!J5)</f>
+        <f>INT('(Criteria) Данные'!J6&lt;='(Criteria) Данные'!J5)</f>
         <v>1</v>
       </c>
       <c r="K6" s="2">
-        <f>INT(Данные!K6&lt;=Данные!K5)</f>
+        <f>INT('(Criteria) Данные'!K6&lt;='(Criteria) Данные'!K5)</f>
         <v>0</v>
       </c>
       <c r="L6" s="2">
-        <f>INT(Данные!L6&lt;=Данные!L5)</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="29">
-        <f>INT(Данные!M6&lt;=Данные!M5)</f>
-        <v>1</v>
-      </c>
-      <c r="N6" s="33"/>
+        <f>INT('(Criteria) Данные'!L6&lt;='(Criteria) Данные'!L5)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="26">
+        <f>INT('(Criteria) Данные'!M6&lt;='(Criteria) Данные'!M5)</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="30"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="33">
+      <c r="B7" s="30">
         <v>2</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="2">
-        <f>INT(Данные!D7&lt;=Данные!D6)</f>
+        <f>INT('(Criteria) Данные'!D7&lt;='(Criteria) Данные'!D6)</f>
         <v>0</v>
       </c>
       <c r="E7" s="2">
-        <f>INT(Данные!E7&lt;=Данные!E6)</f>
+        <f>INT('(Criteria) Данные'!E7&lt;='(Criteria) Данные'!E6)</f>
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <f>INT(Данные!F7&lt;=Данные!F6)</f>
+        <f>INT('(Criteria) Данные'!F7&lt;='(Criteria) Данные'!F6)</f>
         <v>1</v>
       </c>
       <c r="G7" s="2">
-        <f>INT(Данные!G7&lt;=Данные!G6)</f>
+        <f>INT('(Criteria) Данные'!G7&lt;='(Criteria) Данные'!G6)</f>
         <v>1</v>
       </c>
       <c r="H7" s="2">
-        <f>INT(Данные!H7&lt;=Данные!H6)</f>
+        <f>INT('(Criteria) Данные'!H7&lt;='(Criteria) Данные'!H6)</f>
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <f>INT(Данные!I7&lt;=Данные!I6)</f>
+        <f>INT('(Criteria) Данные'!I7&lt;='(Criteria) Данные'!I6)</f>
         <v>0</v>
       </c>
       <c r="J7" s="2">
-        <f>INT(Данные!J7&lt;=Данные!J6)</f>
+        <f>INT('(Criteria) Данные'!J7&lt;='(Criteria) Данные'!J6)</f>
         <v>1</v>
       </c>
       <c r="K7" s="2">
-        <f>INT(Данные!K7&lt;=Данные!K6)</f>
+        <f>INT('(Criteria) Данные'!K7&lt;='(Criteria) Данные'!K6)</f>
         <v>1</v>
       </c>
       <c r="L7" s="2">
-        <f>INT(Данные!L7&lt;=Данные!L6)</f>
-        <v>1</v>
-      </c>
-      <c r="M7" s="29">
-        <f>INT(Данные!M7&lt;=Данные!M6)</f>
-        <v>1</v>
-      </c>
-      <c r="N7" s="33"/>
+        <f>INT('(Criteria) Данные'!L7&lt;='(Criteria) Данные'!L6)</f>
+        <v>1</v>
+      </c>
+      <c r="M7" s="26">
+        <f>INT('(Criteria) Данные'!M7&lt;='(Criteria) Данные'!M6)</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="30"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="33">
+      <c r="B8" s="30">
         <v>3</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="35">
-        <f>INT(Данные!D8&lt;=Данные!D7)</f>
-        <v>1</v>
-      </c>
-      <c r="E8" s="35">
-        <f>INT(Данные!E8&lt;=Данные!E7)</f>
-        <v>1</v>
-      </c>
-      <c r="F8" s="35">
-        <f>INT(Данные!F8&lt;=Данные!F7)</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="35">
-        <f>INT(Данные!G8&lt;=Данные!G7)</f>
-        <v>1</v>
-      </c>
-      <c r="H8" s="35">
-        <f>INT(Данные!H8&lt;=Данные!H7)</f>
-        <v>1</v>
-      </c>
-      <c r="I8" s="35">
-        <f>INT(Данные!I8&lt;=Данные!I7)</f>
-        <v>1</v>
-      </c>
-      <c r="J8" s="37">
-        <f>INT(Данные!J8&lt;=Данные!J7)</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="35">
-        <f>INT(Данные!K8&lt;=Данные!K7)</f>
-        <v>1</v>
-      </c>
-      <c r="L8" s="35">
-        <f>INT(Данные!L8&lt;=Данные!L7)</f>
-        <v>1</v>
-      </c>
-      <c r="M8" s="36">
-        <f>INT(Данные!M8&lt;=Данные!M7)</f>
-        <v>1</v>
-      </c>
-      <c r="N8" s="33"/>
+      <c r="D8" s="32">
+        <f>INT('(Criteria) Данные'!D8&lt;='(Criteria) Данные'!D7)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="32">
+        <f>INT('(Criteria) Данные'!E8&lt;='(Criteria) Данные'!E7)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="32">
+        <f>INT('(Criteria) Данные'!F8&lt;='(Criteria) Данные'!F7)</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="32">
+        <f>INT('(Criteria) Данные'!G8&lt;='(Criteria) Данные'!G7)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="32">
+        <f>INT('(Criteria) Данные'!H8&lt;='(Criteria) Данные'!H7)</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="32">
+        <f>INT('(Criteria) Данные'!I8&lt;='(Criteria) Данные'!I7)</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="34">
+        <f>INT('(Criteria) Данные'!J8&lt;='(Criteria) Данные'!J7)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="32">
+        <f>INT('(Criteria) Данные'!K8&lt;='(Criteria) Данные'!K7)</f>
+        <v>1</v>
+      </c>
+      <c r="L8" s="32">
+        <f>INT('(Criteria) Данные'!L8&lt;='(Criteria) Данные'!L7)</f>
+        <v>1</v>
+      </c>
+      <c r="M8" s="33">
+        <f>INT('(Criteria) Данные'!M8&lt;='(Criteria) Данные'!M7)</f>
+        <v>1</v>
+      </c>
+      <c r="N8" s="30"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="33">
+      <c r="B9" s="30">
         <v>4</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="25" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="2">
-        <f>INT(Данные!D9&lt;=Данные!D8)</f>
+        <f>INT('(Criteria) Данные'!D9&lt;='(Criteria) Данные'!D8)</f>
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <f>INT(Данные!E9&lt;=Данные!E8)</f>
+        <f>INT('(Criteria) Данные'!E9&lt;='(Criteria) Данные'!E8)</f>
         <v>1</v>
       </c>
       <c r="F9" s="2">
-        <f>INT(Данные!F9&lt;=Данные!F8)</f>
+        <f>INT('(Criteria) Данные'!F9&lt;='(Criteria) Данные'!F8)</f>
         <v>0</v>
       </c>
       <c r="G9" s="2">
-        <f>INT(Данные!G9&lt;=Данные!G8)</f>
+        <f>INT('(Criteria) Данные'!G9&lt;='(Criteria) Данные'!G8)</f>
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <f>INT(Данные!H9&lt;=Данные!H8)</f>
+        <f>INT('(Criteria) Данные'!H9&lt;='(Criteria) Данные'!H8)</f>
         <v>1</v>
       </c>
       <c r="I9" s="2">
-        <f>INT(Данные!I9&lt;=Данные!I8)</f>
+        <f>INT('(Criteria) Данные'!I9&lt;='(Criteria) Данные'!I8)</f>
         <v>0</v>
       </c>
       <c r="J9" s="2">
-        <f>INT(Данные!J9&lt;=Данные!J8)</f>
+        <f>INT('(Criteria) Данные'!J9&lt;='(Criteria) Данные'!J8)</f>
         <v>1</v>
       </c>
       <c r="K9" s="2">
-        <f>INT(Данные!K9&lt;=Данные!K8)</f>
+        <f>INT('(Criteria) Данные'!K9&lt;='(Criteria) Данные'!K8)</f>
         <v>0</v>
       </c>
       <c r="L9" s="2">
-        <f>INT(Данные!L9&lt;=Данные!L8)</f>
-        <v>1</v>
-      </c>
-      <c r="M9" s="29">
-        <f>INT(Данные!M9&lt;=Данные!M8)</f>
-        <v>1</v>
-      </c>
-      <c r="N9" s="33"/>
+        <f>INT('(Criteria) Данные'!L9&lt;='(Criteria) Данные'!L8)</f>
+        <v>1</v>
+      </c>
+      <c r="M9" s="26">
+        <f>INT('(Criteria) Данные'!M9&lt;='(Criteria) Данные'!M8)</f>
+        <v>1</v>
+      </c>
+      <c r="N9" s="30"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="33">
+      <c r="B10" s="30">
         <v>5</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="25" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="2">
-        <f>INT(Данные!D10&lt;=Данные!D9)</f>
+        <f>INT('(Criteria) Данные'!D10&lt;='(Criteria) Данные'!D9)</f>
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <f>INT(Данные!E10&lt;=Данные!E9)</f>
+        <f>INT('(Criteria) Данные'!E10&lt;='(Criteria) Данные'!E9)</f>
         <v>1</v>
       </c>
       <c r="F10" s="2">
-        <f>INT(Данные!F10&lt;=Данные!F9)</f>
+        <f>INT('(Criteria) Данные'!F10&lt;='(Criteria) Данные'!F9)</f>
         <v>1</v>
       </c>
       <c r="G10" s="2">
-        <f>INT(Данные!G10&lt;=Данные!G9)</f>
+        <f>INT('(Criteria) Данные'!G10&lt;='(Criteria) Данные'!G9)</f>
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <f>INT(Данные!H10&lt;=Данные!H9)</f>
+        <f>INT('(Criteria) Данные'!H10&lt;='(Criteria) Данные'!H9)</f>
         <v>0</v>
       </c>
       <c r="I10" s="2">
-        <f>INT(Данные!I10&lt;=Данные!I9)</f>
+        <f>INT('(Criteria) Данные'!I10&lt;='(Criteria) Данные'!I9)</f>
         <v>1</v>
       </c>
       <c r="J10" s="2">
-        <f>INT(Данные!J10&lt;=Данные!J9)</f>
+        <f>INT('(Criteria) Данные'!J10&lt;='(Criteria) Данные'!J9)</f>
         <v>0</v>
       </c>
       <c r="K10" s="2">
-        <f>INT(Данные!K10&lt;=Данные!K9)</f>
+        <f>INT('(Criteria) Данные'!K10&lt;='(Criteria) Данные'!K9)</f>
         <v>0</v>
       </c>
       <c r="L10" s="2">
-        <f>INT(Данные!L10&lt;=Данные!L9)</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="29">
-        <f>INT(Данные!M10&lt;=Данные!M9)</f>
-        <v>1</v>
-      </c>
-      <c r="N10" s="33"/>
+        <f>INT('(Criteria) Данные'!L10&lt;='(Criteria) Данные'!L9)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="26">
+        <f>INT('(Criteria) Данные'!M10&lt;='(Criteria) Данные'!M9)</f>
+        <v>1</v>
+      </c>
+      <c r="N10" s="30"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="33">
+      <c r="B11" s="30">
         <v>6</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="2">
-        <f>INT(Данные!D11&lt;=Данные!D10)</f>
+        <f>INT('(Criteria) Данные'!D11&lt;='(Criteria) Данные'!D10)</f>
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <f>INT(Данные!E11&lt;=Данные!E10)</f>
+        <f>INT('(Criteria) Данные'!E11&lt;='(Criteria) Данные'!E10)</f>
         <v>1</v>
       </c>
       <c r="F11" s="2">
-        <f>INT(Данные!F11&lt;=Данные!F10)</f>
+        <f>INT('(Criteria) Данные'!F11&lt;='(Criteria) Данные'!F10)</f>
         <v>0</v>
       </c>
       <c r="G11" s="2">
-        <f>INT(Данные!G11&lt;=Данные!G10)</f>
+        <f>INT('(Criteria) Данные'!G11&lt;='(Criteria) Данные'!G10)</f>
         <v>1</v>
       </c>
       <c r="H11" s="2">
-        <f>INT(Данные!H11&lt;=Данные!H10)</f>
+        <f>INT('(Criteria) Данные'!H11&lt;='(Criteria) Данные'!H10)</f>
         <v>0</v>
       </c>
       <c r="I11" s="2">
-        <f>INT(Данные!I11&lt;=Данные!I10)</f>
+        <f>INT('(Criteria) Данные'!I11&lt;='(Criteria) Данные'!I10)</f>
         <v>1</v>
       </c>
       <c r="J11" s="2">
-        <f>INT(Данные!J11&lt;=Данные!J10)</f>
+        <f>INT('(Criteria) Данные'!J11&lt;='(Criteria) Данные'!J10)</f>
         <v>0</v>
       </c>
       <c r="K11" s="2">
-        <f>INT(Данные!K11&lt;=Данные!K10)</f>
+        <f>INT('(Criteria) Данные'!K11&lt;='(Criteria) Данные'!K10)</f>
         <v>1</v>
       </c>
       <c r="L11" s="2">
-        <f>INT(Данные!L11&lt;=Данные!L10)</f>
-        <v>1</v>
-      </c>
-      <c r="M11" s="29">
-        <f>INT(Данные!M11&lt;=Данные!M10)</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="33"/>
+        <f>INT('(Criteria) Данные'!L11&lt;='(Criteria) Данные'!L10)</f>
+        <v>1</v>
+      </c>
+      <c r="M11" s="26">
+        <f>INT('(Criteria) Данные'!M11&lt;='(Criteria) Данные'!M10)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="30"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="33">
+      <c r="B12" s="30">
         <v>7</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2">
-        <f>INT(Данные!D12&lt;=Данные!D11)</f>
+        <f>INT('(Criteria) Данные'!D12&lt;='(Criteria) Данные'!D11)</f>
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <f>INT(Данные!E12&lt;=Данные!E11)</f>
+        <f>INT('(Criteria) Данные'!E12&lt;='(Criteria) Данные'!E11)</f>
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <f>INT(Данные!F12&lt;=Данные!F11)</f>
+        <f>INT('(Criteria) Данные'!F12&lt;='(Criteria) Данные'!F11)</f>
         <v>1</v>
       </c>
       <c r="G12" s="2">
-        <f>INT(Данные!G12&lt;=Данные!G11)</f>
+        <f>INT('(Criteria) Данные'!G12&lt;='(Criteria) Данные'!G11)</f>
         <v>0</v>
       </c>
       <c r="H12" s="2">
-        <f>INT(Данные!H12&lt;=Данные!H11)</f>
+        <f>INT('(Criteria) Данные'!H12&lt;='(Criteria) Данные'!H11)</f>
         <v>1</v>
       </c>
       <c r="I12" s="2">
-        <f>INT(Данные!I12&lt;=Данные!I11)</f>
+        <f>INT('(Criteria) Данные'!I12&lt;='(Criteria) Данные'!I11)</f>
         <v>0</v>
       </c>
       <c r="J12" s="2">
-        <f>INT(Данные!J12&lt;=Данные!J11)</f>
+        <f>INT('(Criteria) Данные'!J12&lt;='(Criteria) Данные'!J11)</f>
         <v>1</v>
       </c>
       <c r="K12" s="2">
-        <f>INT(Данные!K12&lt;=Данные!K11)</f>
+        <f>INT('(Criteria) Данные'!K12&lt;='(Criteria) Данные'!K11)</f>
         <v>1</v>
       </c>
       <c r="L12" s="2">
-        <f>INT(Данные!L12&lt;=Данные!L11)</f>
-        <v>1</v>
-      </c>
-      <c r="M12" s="29">
-        <f>INT(Данные!M12&lt;=Данные!M11)</f>
-        <v>1</v>
-      </c>
-      <c r="N12" s="33"/>
+        <f>INT('(Criteria) Данные'!L12&lt;='(Criteria) Данные'!L11)</f>
+        <v>1</v>
+      </c>
+      <c r="M12" s="26">
+        <f>INT('(Criteria) Данные'!M12&lt;='(Criteria) Данные'!M11)</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="33">
+      <c r="B13" s="30">
         <v>8</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="25" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="2">
-        <f>INT(Данные!D13&lt;=Данные!D12)</f>
+        <f>INT('(Criteria) Данные'!D13&lt;='(Criteria) Данные'!D12)</f>
         <v>0</v>
       </c>
       <c r="E13" s="2">
-        <f>INT(Данные!E13&lt;=Данные!E12)</f>
+        <f>INT('(Criteria) Данные'!E13&lt;='(Criteria) Данные'!E12)</f>
         <v>1</v>
       </c>
       <c r="F13" s="2">
-        <f>INT(Данные!F13&lt;=Данные!F12)</f>
+        <f>INT('(Criteria) Данные'!F13&lt;='(Criteria) Данные'!F12)</f>
         <v>1</v>
       </c>
       <c r="G13" s="2">
-        <f>INT(Данные!G13&lt;=Данные!G12)</f>
+        <f>INT('(Criteria) Данные'!G13&lt;='(Criteria) Данные'!G12)</f>
         <v>0</v>
       </c>
       <c r="H13" s="2">
-        <f>INT(Данные!H13&lt;=Данные!H12)</f>
+        <f>INT('(Criteria) Данные'!H13&lt;='(Criteria) Данные'!H12)</f>
         <v>0</v>
       </c>
       <c r="I13" s="2">
-        <f>INT(Данные!I13&lt;=Данные!I12)</f>
+        <f>INT('(Criteria) Данные'!I13&lt;='(Criteria) Данные'!I12)</f>
         <v>0</v>
       </c>
       <c r="J13" s="2">
-        <f>INT(Данные!J13&lt;=Данные!J12)</f>
+        <f>INT('(Criteria) Данные'!J13&lt;='(Criteria) Данные'!J12)</f>
         <v>1</v>
       </c>
       <c r="K13" s="2">
-        <f>INT(Данные!K13&lt;=Данные!K12)</f>
+        <f>INT('(Criteria) Данные'!K13&lt;='(Criteria) Данные'!K12)</f>
         <v>0</v>
       </c>
       <c r="L13" s="2">
-        <f>INT(Данные!L13&lt;=Данные!L12)</f>
-        <v>1</v>
-      </c>
-      <c r="M13" s="29">
-        <f>INT(Данные!M13&lt;=Данные!M12)</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="33"/>
+        <f>INT('(Criteria) Данные'!L13&lt;='(Criteria) Данные'!L12)</f>
+        <v>1</v>
+      </c>
+      <c r="M13" s="26">
+        <f>INT('(Criteria) Данные'!M13&lt;='(Criteria) Данные'!M12)</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="30"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="33">
+      <c r="B14" s="30">
         <v>9</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="2">
-        <f>INT(Данные!D14&lt;=Данные!D13)</f>
+        <f>INT('(Criteria) Данные'!D14&lt;='(Criteria) Данные'!D13)</f>
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <f>INT(Данные!E14&lt;=Данные!E13)</f>
+        <f>INT('(Criteria) Данные'!E14&lt;='(Criteria) Данные'!E13)</f>
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <f>INT(Данные!F14&lt;=Данные!F13)</f>
+        <f>INT('(Criteria) Данные'!F14&lt;='(Criteria) Данные'!F13)</f>
         <v>1</v>
       </c>
       <c r="G14" s="2">
-        <f>INT(Данные!G14&lt;=Данные!G13)</f>
+        <f>INT('(Criteria) Данные'!G14&lt;='(Criteria) Данные'!G13)</f>
         <v>1</v>
       </c>
       <c r="H14" s="2">
-        <f>INT(Данные!H14&lt;=Данные!H13)</f>
+        <f>INT('(Criteria) Данные'!H14&lt;='(Criteria) Данные'!H13)</f>
         <v>1</v>
       </c>
       <c r="I14" s="2">
-        <f>INT(Данные!I14&lt;=Данные!I13)</f>
+        <f>INT('(Criteria) Данные'!I14&lt;='(Criteria) Данные'!I13)</f>
         <v>1</v>
       </c>
       <c r="J14" s="2">
-        <f>INT(Данные!J14&lt;=Данные!J13)</f>
+        <f>INT('(Criteria) Данные'!J14&lt;='(Criteria) Данные'!J13)</f>
         <v>0</v>
       </c>
       <c r="K14" s="2">
-        <f>INT(Данные!K14&lt;=Данные!K13)</f>
+        <f>INT('(Criteria) Данные'!K14&lt;='(Criteria) Данные'!K13)</f>
         <v>0</v>
       </c>
       <c r="L14" s="2">
-        <f>INT(Данные!L14&lt;=Данные!L13)</f>
-        <v>1</v>
-      </c>
-      <c r="M14" s="29">
-        <f>INT(Данные!M14&lt;=Данные!M13)</f>
-        <v>1</v>
-      </c>
-      <c r="N14" s="33"/>
+        <f>INT('(Criteria) Данные'!L14&lt;='(Criteria) Данные'!L13)</f>
+        <v>1</v>
+      </c>
+      <c r="M14" s="26">
+        <f>INT('(Criteria) Данные'!M14&lt;='(Criteria) Данные'!M13)</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="33">
+      <c r="B15" s="30">
         <v>10</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="2">
-        <f>INT(Данные!D15&lt;=Данные!D14)</f>
+        <f>INT('(Criteria) Данные'!D15&lt;='(Criteria) Данные'!D14)</f>
         <v>0</v>
       </c>
       <c r="E15" s="2">
-        <f>INT(Данные!E15&lt;=Данные!E14)</f>
+        <f>INT('(Criteria) Данные'!E15&lt;='(Criteria) Данные'!E14)</f>
         <v>1</v>
       </c>
       <c r="F15" s="2">
-        <f>INT(Данные!F15&lt;=Данные!F14)</f>
+        <f>INT('(Criteria) Данные'!F15&lt;='(Criteria) Данные'!F14)</f>
         <v>0</v>
       </c>
       <c r="G15" s="2">
-        <f>INT(Данные!G15&lt;=Данные!G14)</f>
+        <f>INT('(Criteria) Данные'!G15&lt;='(Criteria) Данные'!G14)</f>
         <v>0</v>
       </c>
       <c r="H15" s="2">
-        <f>INT(Данные!H15&lt;=Данные!H14)</f>
+        <f>INT('(Criteria) Данные'!H15&lt;='(Criteria) Данные'!H14)</f>
         <v>0</v>
       </c>
       <c r="I15" s="2">
-        <f>INT(Данные!I15&lt;=Данные!I14)</f>
+        <f>INT('(Criteria) Данные'!I15&lt;='(Criteria) Данные'!I14)</f>
         <v>0</v>
       </c>
       <c r="J15" s="2">
-        <f>INT(Данные!J15&lt;=Данные!J14)</f>
+        <f>INT('(Criteria) Данные'!J15&lt;='(Criteria) Данные'!J14)</f>
         <v>1</v>
       </c>
       <c r="K15" s="2">
-        <f>INT(Данные!K15&lt;=Данные!K14)</f>
+        <f>INT('(Criteria) Данные'!K15&lt;='(Criteria) Данные'!K14)</f>
         <v>1</v>
       </c>
       <c r="L15" s="2">
-        <f>INT(Данные!L15&lt;=Данные!L14)</f>
-        <v>1</v>
-      </c>
-      <c r="M15" s="29">
-        <f>INT(Данные!M15&lt;=Данные!M14)</f>
-        <v>1</v>
-      </c>
-      <c r="N15" s="33"/>
+        <f>INT('(Criteria) Данные'!L15&lt;='(Criteria) Данные'!L14)</f>
+        <v>1</v>
+      </c>
+      <c r="M15" s="26">
+        <f>INT('(Criteria) Данные'!M15&lt;='(Criteria) Данные'!M14)</f>
+        <v>1</v>
+      </c>
+      <c r="N15" s="30"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="33">
+      <c r="B16" s="30">
         <v>11</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="25" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="2">
-        <f>INT(Данные!D16&lt;=Данные!D15)</f>
+        <f>INT('(Criteria) Данные'!D16&lt;='(Criteria) Данные'!D15)</f>
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <f>INT(Данные!E16&lt;=Данные!E15)</f>
+        <f>INT('(Criteria) Данные'!E16&lt;='(Criteria) Данные'!E15)</f>
         <v>1</v>
       </c>
       <c r="F16" s="2">
-        <f>INT(Данные!F16&lt;=Данные!F15)</f>
+        <f>INT('(Criteria) Данные'!F16&lt;='(Criteria) Данные'!F15)</f>
         <v>1</v>
       </c>
       <c r="G16" s="2">
-        <f>INT(Данные!G16&lt;=Данные!G15)</f>
+        <f>INT('(Criteria) Данные'!G16&lt;='(Criteria) Данные'!G15)</f>
         <v>1</v>
       </c>
       <c r="H16" s="2">
-        <f>INT(Данные!H16&lt;=Данные!H15)</f>
+        <f>INT('(Criteria) Данные'!H16&lt;='(Criteria) Данные'!H15)</f>
         <v>0</v>
       </c>
       <c r="I16" s="2">
-        <f>INT(Данные!I16&lt;=Данные!I15)</f>
+        <f>INT('(Criteria) Данные'!I16&lt;='(Criteria) Данные'!I15)</f>
         <v>0</v>
       </c>
       <c r="J16" s="2">
-        <f>INT(Данные!J16&lt;=Данные!J15)</f>
+        <f>INT('(Criteria) Данные'!J16&lt;='(Criteria) Данные'!J15)</f>
         <v>0</v>
       </c>
       <c r="K16" s="2">
-        <f>INT(Данные!K16&lt;=Данные!K15)</f>
+        <f>INT('(Criteria) Данные'!K16&lt;='(Criteria) Данные'!K15)</f>
         <v>0</v>
       </c>
       <c r="L16" s="2">
-        <f>INT(Данные!L16&lt;=Данные!L15)</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="29">
-        <f>INT(Данные!M16&lt;=Данные!M15)</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="33"/>
+        <f>INT('(Criteria) Данные'!L16&lt;='(Criteria) Данные'!L15)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="26">
+        <f>INT('(Criteria) Данные'!M16&lt;='(Criteria) Данные'!M15)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="30"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="33">
+      <c r="B17" s="30">
         <v>12</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="25" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="2">
-        <f>INT(Данные!D17&lt;=Данные!D16)</f>
+        <f>INT('(Criteria) Данные'!D17&lt;='(Criteria) Данные'!D16)</f>
         <v>0</v>
       </c>
       <c r="E17" s="2">
-        <f>INT(Данные!E17&lt;=Данные!E16)</f>
+        <f>INT('(Criteria) Данные'!E17&lt;='(Criteria) Данные'!E16)</f>
         <v>0</v>
       </c>
       <c r="F17" s="2">
-        <f>INT(Данные!F17&lt;=Данные!F16)</f>
+        <f>INT('(Criteria) Данные'!F17&lt;='(Criteria) Данные'!F16)</f>
         <v>0</v>
       </c>
       <c r="G17" s="2">
-        <f>INT(Данные!G17&lt;=Данные!G16)</f>
+        <f>INT('(Criteria) Данные'!G17&lt;='(Criteria) Данные'!G16)</f>
         <v>0</v>
       </c>
       <c r="H17" s="2">
-        <f>INT(Данные!H17&lt;=Данные!H16)</f>
+        <f>INT('(Criteria) Данные'!H17&lt;='(Criteria) Данные'!H16)</f>
         <v>1</v>
       </c>
       <c r="I17" s="2">
-        <f>INT(Данные!I17&lt;=Данные!I16)</f>
+        <f>INT('(Criteria) Данные'!I17&lt;='(Criteria) Данные'!I16)</f>
         <v>1</v>
       </c>
       <c r="J17" s="2">
-        <f>INT(Данные!J17&lt;=Данные!J16)</f>
+        <f>INT('(Criteria) Данные'!J17&lt;='(Criteria) Данные'!J16)</f>
         <v>1</v>
       </c>
       <c r="K17" s="2">
-        <f>INT(Данные!K17&lt;=Данные!K16)</f>
+        <f>INT('(Criteria) Данные'!K17&lt;='(Criteria) Данные'!K16)</f>
         <v>1</v>
       </c>
       <c r="L17" s="2">
-        <f>INT(Данные!L17&lt;=Данные!L16)</f>
-        <v>1</v>
-      </c>
-      <c r="M17" s="29">
-        <f>INT(Данные!M17&lt;=Данные!M16)</f>
-        <v>1</v>
-      </c>
-      <c r="N17" s="33"/>
+        <f>INT('(Criteria) Данные'!L17&lt;='(Criteria) Данные'!L16)</f>
+        <v>1</v>
+      </c>
+      <c r="M17" s="26">
+        <f>INT('(Criteria) Данные'!M17&lt;='(Criteria) Данные'!M16)</f>
+        <v>1</v>
+      </c>
+      <c r="N17" s="30"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="33">
+      <c r="B18" s="30">
         <v>13</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="25" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="2">
-        <f>INT(Данные!D18&lt;=Данные!D17)</f>
+        <f>INT('(Criteria) Данные'!D18&lt;='(Criteria) Данные'!D17)</f>
         <v>1</v>
       </c>
       <c r="E18" s="2">
-        <f>INT(Данные!E18&lt;=Данные!E17)</f>
+        <f>INT('(Criteria) Данные'!E18&lt;='(Criteria) Данные'!E17)</f>
         <v>1</v>
       </c>
       <c r="F18" s="2">
-        <f>INT(Данные!F18&lt;=Данные!F17)</f>
+        <f>INT('(Criteria) Данные'!F18&lt;='(Criteria) Данные'!F17)</f>
         <v>1</v>
       </c>
       <c r="G18" s="2">
-        <f>INT(Данные!G18&lt;=Данные!G17)</f>
+        <f>INT('(Criteria) Данные'!G18&lt;='(Criteria) Данные'!G17)</f>
         <v>1</v>
       </c>
       <c r="H18" s="2">
-        <f>INT(Данные!H18&lt;=Данные!H17)</f>
+        <f>INT('(Criteria) Данные'!H18&lt;='(Criteria) Данные'!H17)</f>
         <v>0</v>
       </c>
       <c r="I18" s="2">
-        <f>INT(Данные!I18&lt;=Данные!I17)</f>
+        <f>INT('(Criteria) Данные'!I18&lt;='(Criteria) Данные'!I17)</f>
         <v>1</v>
       </c>
       <c r="J18" s="2">
-        <f>INT(Данные!J18&lt;=Данные!J17)</f>
+        <f>INT('(Criteria) Данные'!J18&lt;='(Criteria) Данные'!J17)</f>
         <v>0</v>
       </c>
       <c r="K18" s="2">
-        <f>INT(Данные!K18&lt;=Данные!K17)</f>
+        <f>INT('(Criteria) Данные'!K18&lt;='(Criteria) Данные'!K17)</f>
         <v>1</v>
       </c>
       <c r="L18" s="2">
-        <f>INT(Данные!L18&lt;=Данные!L17)</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="29">
-        <f>INT(Данные!M18&lt;=Данные!M17)</f>
-        <v>1</v>
-      </c>
-      <c r="N18" s="33"/>
+        <f>INT('(Criteria) Данные'!L18&lt;='(Criteria) Данные'!L17)</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="26">
+        <f>INT('(Criteria) Данные'!M18&lt;='(Criteria) Данные'!M17)</f>
+        <v>1</v>
+      </c>
+      <c r="N18" s="30"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="33">
+      <c r="B19" s="30">
         <v>14</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="2">
-        <f>INT(Данные!D19&lt;=Данные!D18)</f>
+        <f>INT('(Criteria) Данные'!D19&lt;='(Criteria) Данные'!D18)</f>
         <v>1</v>
       </c>
       <c r="E19" s="2">
-        <f>INT(Данные!E19&lt;=Данные!E18)</f>
+        <f>INT('(Criteria) Данные'!E19&lt;='(Criteria) Данные'!E18)</f>
         <v>1</v>
       </c>
       <c r="F19" s="2">
-        <f>INT(Данные!F19&lt;=Данные!F18)</f>
+        <f>INT('(Criteria) Данные'!F19&lt;='(Criteria) Данные'!F18)</f>
         <v>1</v>
       </c>
       <c r="G19" s="2">
-        <f>INT(Данные!G19&lt;=Данные!G18)</f>
+        <f>INT('(Criteria) Данные'!G19&lt;='(Criteria) Данные'!G18)</f>
         <v>0</v>
       </c>
       <c r="H19" s="2">
-        <f>INT(Данные!H19&lt;=Данные!H18)</f>
+        <f>INT('(Criteria) Данные'!H19&lt;='(Criteria) Данные'!H18)</f>
         <v>1</v>
       </c>
       <c r="I19" s="2">
-        <f>INT(Данные!I19&lt;=Данные!I18)</f>
+        <f>INT('(Criteria) Данные'!I19&lt;='(Criteria) Данные'!I18)</f>
         <v>0</v>
       </c>
       <c r="J19" s="2">
-        <f>INT(Данные!J19&lt;=Данные!J18)</f>
+        <f>INT('(Criteria) Данные'!J19&lt;='(Criteria) Данные'!J18)</f>
         <v>1</v>
       </c>
       <c r="K19" s="2">
-        <f>INT(Данные!K19&lt;=Данные!K18)</f>
+        <f>INT('(Criteria) Данные'!K19&lt;='(Criteria) Данные'!K18)</f>
         <v>0</v>
       </c>
       <c r="L19" s="2">
-        <f>INT(Данные!L19&lt;=Данные!L18)</f>
-        <v>1</v>
-      </c>
-      <c r="M19" s="29">
-        <f>INT(Данные!M19&lt;=Данные!M18)</f>
-        <v>1</v>
-      </c>
-      <c r="N19" s="33"/>
+        <f>INT('(Criteria) Данные'!L19&lt;='(Criteria) Данные'!L18)</f>
+        <v>1</v>
+      </c>
+      <c r="M19" s="26">
+        <f>INT('(Criteria) Данные'!M19&lt;='(Criteria) Данные'!M18)</f>
+        <v>1</v>
+      </c>
+      <c r="N19" s="30"/>
     </row>
     <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="33">
+      <c r="B20" s="30">
         <v>15</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="31">
-        <f>INT(Данные!D20&lt;=Данные!D19)</f>
-        <v>1</v>
-      </c>
-      <c r="E20" s="31">
-        <f>INT(Данные!E20&lt;=Данные!E19)</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="31">
-        <f>INT(Данные!F20&lt;=Данные!F19)</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="31">
-        <f>INT(Данные!G20&lt;=Данные!G19)</f>
-        <v>1</v>
-      </c>
-      <c r="H20" s="31">
-        <f>INT(Данные!H20&lt;=Данные!H19)</f>
-        <v>1</v>
-      </c>
-      <c r="I20" s="31">
-        <f>INT(Данные!I20&lt;=Данные!I19)</f>
-        <v>1</v>
-      </c>
-      <c r="J20" s="31">
-        <f>INT(Данные!J20&lt;=Данные!J19)</f>
-        <v>1</v>
-      </c>
-      <c r="K20" s="31">
-        <f>INT(Данные!K20&lt;=Данные!K19)</f>
-        <v>1</v>
-      </c>
-      <c r="L20" s="31">
-        <f>INT(Данные!L20&lt;=Данные!L19)</f>
-        <v>1</v>
-      </c>
-      <c r="M20" s="32">
-        <f>INT(Данные!M20&lt;=Данные!M19)</f>
-        <v>0</v>
-      </c>
-      <c r="N20" s="33"/>
+      <c r="D20" s="28">
+        <f>INT('(Criteria) Данные'!D20&lt;='(Criteria) Данные'!D19)</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="28">
+        <f>INT('(Criteria) Данные'!E20&lt;='(Criteria) Данные'!E19)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="28">
+        <f>INT('(Criteria) Данные'!F20&lt;='(Criteria) Данные'!F19)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="28">
+        <f>INT('(Criteria) Данные'!G20&lt;='(Criteria) Данные'!G19)</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="28">
+        <f>INT('(Criteria) Данные'!H20&lt;='(Criteria) Данные'!H19)</f>
+        <v>1</v>
+      </c>
+      <c r="I20" s="28">
+        <f>INT('(Criteria) Данные'!I20&lt;='(Criteria) Данные'!I19)</f>
+        <v>1</v>
+      </c>
+      <c r="J20" s="28">
+        <f>INT('(Criteria) Данные'!J20&lt;='(Criteria) Данные'!J19)</f>
+        <v>1</v>
+      </c>
+      <c r="K20" s="28">
+        <f>INT('(Criteria) Данные'!K20&lt;='(Criteria) Данные'!K19)</f>
+        <v>1</v>
+      </c>
+      <c r="L20" s="28">
+        <f>INT('(Criteria) Данные'!L20&lt;='(Criteria) Данные'!L19)</f>
+        <v>1</v>
+      </c>
+      <c r="M20" s="29">
+        <f>INT('(Criteria) Данные'!M20&lt;='(Criteria) Данные'!M19)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="30"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2599,19 +2711,19 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="33"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="18" t="s">
         <v>46</v>
       </c>
@@ -2636,11 +2748,11 @@
       <c r="J5" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="K5" s="34"/>
+      <c r="K5" s="31"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="14" t="s">
         <v>15</v>
       </c>
@@ -2666,10 +2778,10 @@
       <c r="J6" s="17">
         <v>1</v>
       </c>
-      <c r="K6" s="33"/>
+      <c r="K6" s="30"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="33"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
@@ -2700,10 +2812,10 @@
       <c r="J7" s="9">
         <v>6</v>
       </c>
-      <c r="K7" s="33"/>
+      <c r="K7" s="30"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
@@ -2734,10 +2846,10 @@
       <c r="J8" s="9">
         <v>6</v>
       </c>
-      <c r="K8" s="33"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="33"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -2767,10 +2879,10 @@
       <c r="J9" s="9">
         <v>5</v>
       </c>
-      <c r="K9" s="33"/>
+      <c r="K9" s="30"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="8" t="s">
         <v>23</v>
       </c>
@@ -2798,10 +2910,10 @@
       <c r="J10" s="9">
         <v>3</v>
       </c>
-      <c r="K10" s="33"/>
+      <c r="K10" s="30"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="33"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="8" t="s">
         <v>25</v>
       </c>
@@ -2832,10 +2944,10 @@
       <c r="J11" s="9">
         <v>6</v>
       </c>
-      <c r="K11" s="33"/>
+      <c r="K11" s="30"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="33"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="8" t="s">
         <v>27</v>
       </c>
@@ -2866,10 +2978,10 @@
       <c r="J12" s="9">
         <v>6</v>
       </c>
-      <c r="K12" s="33"/>
+      <c r="K12" s="30"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="8" t="s">
         <v>29</v>
       </c>
@@ -2896,10 +3008,10 @@
       <c r="J13" s="9">
         <v>2</v>
       </c>
-      <c r="K13" s="33"/>
+      <c r="K13" s="30"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="33"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="8" t="s">
         <v>31</v>
       </c>
@@ -2930,10 +3042,10 @@
       <c r="J14" s="9">
         <v>6</v>
       </c>
-      <c r="K14" s="33"/>
+      <c r="K14" s="30"/>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="33"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="10" t="s">
         <v>32</v>
       </c>
@@ -2962,19 +3074,19 @@
       <c r="J15" s="13">
         <v>4</v>
       </c>
-      <c r="K15" s="33"/>
+      <c r="K15" s="30"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2984,4 +3096,1753 @@
     <ignoredError sqref="D12" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47085B6B-A0C8-470C-BF16-E059821430EF}">
+  <dimension ref="B6:K24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:11" ht="109.5" x14ac:dyDescent="0.25">
+      <c r="C7" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="42"/>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="43"/>
+      <c r="D9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="38">
+        <v>13.2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>14</v>
+      </c>
+      <c r="H10" s="38">
+        <v>25</v>
+      </c>
+      <c r="I10" s="38">
+        <v>11.45</v>
+      </c>
+      <c r="J10" s="2">
+        <v>65</v>
+      </c>
+      <c r="K10" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="38">
+        <v>14</v>
+      </c>
+      <c r="E11" s="38">
+        <v>10</v>
+      </c>
+      <c r="F11" s="38">
+        <v>1</v>
+      </c>
+      <c r="G11" s="38">
+        <v>5</v>
+      </c>
+      <c r="H11" s="38">
+        <v>37.5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>12.45</v>
+      </c>
+      <c r="J11" s="2">
+        <v>65</v>
+      </c>
+      <c r="K11" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="38">
+        <v>11.5</v>
+      </c>
+      <c r="E12" s="38">
+        <v>10</v>
+      </c>
+      <c r="F12" s="38">
+        <v>1</v>
+      </c>
+      <c r="G12" s="38">
+        <v>5</v>
+      </c>
+      <c r="H12" s="38">
+        <v>25</v>
+      </c>
+      <c r="I12" s="38">
+        <v>10.75</v>
+      </c>
+      <c r="J12" s="38">
+        <v>60</v>
+      </c>
+      <c r="K12" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>4</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="38">
+        <v>12.5</v>
+      </c>
+      <c r="E13" s="38">
+        <v>10</v>
+      </c>
+      <c r="F13" s="38">
+        <v>1.2</v>
+      </c>
+      <c r="G13" s="38">
+        <v>4</v>
+      </c>
+      <c r="H13" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="I13" s="2">
+        <v>11.6</v>
+      </c>
+      <c r="J13" s="2">
+        <v>65</v>
+      </c>
+      <c r="K13" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>5</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="38">
+        <v>12</v>
+      </c>
+      <c r="E14" s="38">
+        <v>10</v>
+      </c>
+      <c r="F14" s="38">
+        <v>0</v>
+      </c>
+      <c r="G14" s="38">
+        <v>18</v>
+      </c>
+      <c r="H14" s="38">
+        <v>25</v>
+      </c>
+      <c r="I14" s="38">
+        <v>10.75</v>
+      </c>
+      <c r="J14" s="38">
+        <v>75</v>
+      </c>
+      <c r="K14" s="40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>6</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="38">
+        <v>7.05</v>
+      </c>
+      <c r="E15" s="38">
+        <v>5</v>
+      </c>
+      <c r="F15" s="38">
+        <v>1</v>
+      </c>
+      <c r="G15" s="38">
+        <v>1</v>
+      </c>
+      <c r="H15" s="38">
+        <v>37.5</v>
+      </c>
+      <c r="I15" s="38">
+        <v>5.5250000000000004</v>
+      </c>
+      <c r="J15" s="38">
+        <v>69</v>
+      </c>
+      <c r="K15" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>7</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="38">
+        <v>11</v>
+      </c>
+      <c r="E16" s="38">
+        <v>15</v>
+      </c>
+      <c r="F16" s="38">
+        <v>1</v>
+      </c>
+      <c r="G16" s="38">
+        <v>3</v>
+      </c>
+      <c r="H16" s="38">
+        <v>7.5</v>
+      </c>
+      <c r="I16" s="38">
+        <v>9.5</v>
+      </c>
+      <c r="J16" s="38">
+        <v>55</v>
+      </c>
+      <c r="K16" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>8</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="38">
+        <v>13</v>
+      </c>
+      <c r="E17" s="38">
+        <v>0</v>
+      </c>
+      <c r="F17" s="38">
+        <v>1</v>
+      </c>
+      <c r="G17" s="38">
+        <v>5</v>
+      </c>
+      <c r="H17" s="38">
+        <v>25</v>
+      </c>
+      <c r="I17" s="38">
+        <v>11</v>
+      </c>
+      <c r="J17" s="38">
+        <v>60</v>
+      </c>
+      <c r="K17" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="5">
+        <v>9</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="38">
+        <v>11</v>
+      </c>
+      <c r="E18" s="38">
+        <v>30</v>
+      </c>
+      <c r="F18" s="38">
+        <v>0</v>
+      </c>
+      <c r="G18" s="38">
+        <v>1</v>
+      </c>
+      <c r="H18" s="38">
+        <v>7.5</v>
+      </c>
+      <c r="I18" s="38">
+        <v>10</v>
+      </c>
+      <c r="J18" s="38">
+        <v>70</v>
+      </c>
+      <c r="K18" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>10</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="38">
+        <v>11.5</v>
+      </c>
+      <c r="E19" s="38">
+        <v>15</v>
+      </c>
+      <c r="F19" s="38">
+        <v>1</v>
+      </c>
+      <c r="G19" s="38">
+        <v>5</v>
+      </c>
+      <c r="H19" s="38">
+        <v>12.5</v>
+      </c>
+      <c r="I19" s="38">
+        <v>10.25</v>
+      </c>
+      <c r="J19" s="38">
+        <v>60</v>
+      </c>
+      <c r="K19" s="40">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <v>11</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="38">
+        <v>11.8</v>
+      </c>
+      <c r="E20" s="38">
+        <v>10</v>
+      </c>
+      <c r="F20" s="38">
+        <v>0.8</v>
+      </c>
+      <c r="G20" s="38">
+        <v>5</v>
+      </c>
+      <c r="H20" s="38">
+        <v>50</v>
+      </c>
+      <c r="I20" s="38">
+        <v>10.65</v>
+      </c>
+      <c r="J20" s="38">
+        <v>70</v>
+      </c>
+      <c r="K20" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>12</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="38">
+        <v>11.9</v>
+      </c>
+      <c r="E21" s="38">
+        <v>15</v>
+      </c>
+      <c r="F21" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="G21" s="38">
+        <v>7</v>
+      </c>
+      <c r="H21" s="38">
+        <v>37.5</v>
+      </c>
+      <c r="I21" s="38">
+        <v>10.45</v>
+      </c>
+      <c r="J21" s="38">
+        <v>60</v>
+      </c>
+      <c r="K21" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>13</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="38">
+        <v>11.5</v>
+      </c>
+      <c r="E22" s="38">
+        <v>15</v>
+      </c>
+      <c r="F22" s="38">
+        <v>0.8</v>
+      </c>
+      <c r="G22" s="38">
+        <v>3</v>
+      </c>
+      <c r="H22" s="38">
+        <v>50</v>
+      </c>
+      <c r="I22" s="38">
+        <v>10.25</v>
+      </c>
+      <c r="J22" s="38">
+        <v>54</v>
+      </c>
+      <c r="K22" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <v>14</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="38">
+        <v>11.5</v>
+      </c>
+      <c r="E23" s="38">
+        <v>10</v>
+      </c>
+      <c r="F23" s="38">
+        <v>0</v>
+      </c>
+      <c r="G23" s="38">
+        <v>5</v>
+      </c>
+      <c r="H23" s="38">
+        <v>12.5</v>
+      </c>
+      <c r="I23" s="38">
+        <v>10.5</v>
+      </c>
+      <c r="J23" s="38">
+        <v>60</v>
+      </c>
+      <c r="K23" s="40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>15</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="39">
+        <v>10.5</v>
+      </c>
+      <c r="E24" s="39">
+        <v>25</v>
+      </c>
+      <c r="F24" s="28">
+        <v>3</v>
+      </c>
+      <c r="G24" s="28">
+        <v>5</v>
+      </c>
+      <c r="H24" s="28">
+        <v>7.5</v>
+      </c>
+      <c r="I24" s="28">
+        <v>9.625</v>
+      </c>
+      <c r="J24" s="28">
+        <v>60</v>
+      </c>
+      <c r="K24" s="29">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C7:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F66624-DBED-43C6-BC18-B91A3DB8C019}">
+  <dimension ref="A1:T29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="18" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+    </row>
+    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+    </row>
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="47">
+        <v>1</v>
+      </c>
+      <c r="E8" s="48">
+        <v>2</v>
+      </c>
+      <c r="F8" s="48">
+        <v>3</v>
+      </c>
+      <c r="G8" s="48">
+        <v>4</v>
+      </c>
+      <c r="H8" s="48">
+        <v>5</v>
+      </c>
+      <c r="I8" s="48">
+        <v>6</v>
+      </c>
+      <c r="J8" s="48">
+        <v>7</v>
+      </c>
+      <c r="K8" s="48">
+        <v>8</v>
+      </c>
+      <c r="L8" s="48">
+        <v>9</v>
+      </c>
+      <c r="M8" s="48">
+        <v>10</v>
+      </c>
+      <c r="N8" s="48">
+        <v>11</v>
+      </c>
+      <c r="O8" s="48">
+        <v>12</v>
+      </c>
+      <c r="P8" s="48">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="48">
+        <v>14</v>
+      </c>
+      <c r="R8" s="49">
+        <v>15</v>
+      </c>
+      <c r="S8" s="30"/>
+      <c r="T8" s="30"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="50">
+        <v>1</v>
+      </c>
+      <c r="D9" s="44">
+        <v>0</v>
+      </c>
+      <c r="E9" s="45">
+        <v>0</v>
+      </c>
+      <c r="F9" s="45">
+        <v>0</v>
+      </c>
+      <c r="G9" s="45">
+        <v>0</v>
+      </c>
+      <c r="H9" s="45">
+        <v>0</v>
+      </c>
+      <c r="I9" s="45">
+        <v>0</v>
+      </c>
+      <c r="J9" s="45">
+        <v>0</v>
+      </c>
+      <c r="K9" s="45">
+        <v>0</v>
+      </c>
+      <c r="L9" s="45">
+        <v>0</v>
+      </c>
+      <c r="M9" s="45">
+        <v>0</v>
+      </c>
+      <c r="N9" s="45">
+        <v>0</v>
+      </c>
+      <c r="O9" s="45">
+        <v>0</v>
+      </c>
+      <c r="P9" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="45">
+        <v>0</v>
+      </c>
+      <c r="R9" s="46">
+        <v>0</v>
+      </c>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="51">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+      <c r="O10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>0</v>
+      </c>
+      <c r="R10" s="9">
+        <v>0</v>
+      </c>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="51">
+        <v>3</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="6">
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+      <c r="O11" s="6">
+        <v>0</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0</v>
+      </c>
+      <c r="R11" s="9">
+        <v>0</v>
+      </c>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="51">
+        <v>4</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0</v>
+      </c>
+      <c r="O12" s="6">
+        <v>0</v>
+      </c>
+      <c r="P12" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>0</v>
+      </c>
+      <c r="R12" s="9">
+        <v>0</v>
+      </c>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="51">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
+        <v>0</v>
+      </c>
+      <c r="M13" s="6">
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0</v>
+      </c>
+      <c r="P13" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>0</v>
+      </c>
+      <c r="R13" s="9">
+        <v>0</v>
+      </c>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="51">
+        <v>6</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="6">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0</v>
+      </c>
+      <c r="O14" s="6">
+        <v>0</v>
+      </c>
+      <c r="P14" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>0</v>
+      </c>
+      <c r="R14" s="9">
+        <v>0</v>
+      </c>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="51">
+        <v>7</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
+      <c r="J15" s="6">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="L15" s="6">
+        <v>0</v>
+      </c>
+      <c r="M15" s="6">
+        <v>0</v>
+      </c>
+      <c r="N15" s="6">
+        <v>0</v>
+      </c>
+      <c r="O15" s="6">
+        <v>0</v>
+      </c>
+      <c r="P15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>0</v>
+      </c>
+      <c r="R15" s="9">
+        <v>0</v>
+      </c>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="51">
+        <v>8</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6">
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
+        <v>0</v>
+      </c>
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>0</v>
+      </c>
+      <c r="R16" s="9">
+        <v>0</v>
+      </c>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="51">
+        <v>9</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0</v>
+      </c>
+      <c r="J17" s="6">
+        <v>0</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0</v>
+      </c>
+      <c r="L17" s="6">
+        <v>0</v>
+      </c>
+      <c r="M17" s="6">
+        <v>0</v>
+      </c>
+      <c r="N17" s="6">
+        <v>0</v>
+      </c>
+      <c r="O17" s="6">
+        <v>0</v>
+      </c>
+      <c r="P17" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>0</v>
+      </c>
+      <c r="R17" s="9">
+        <v>0</v>
+      </c>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="51">
+        <v>10</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0</v>
+      </c>
+      <c r="L18" s="6">
+        <v>0</v>
+      </c>
+      <c r="M18" s="6">
+        <v>0</v>
+      </c>
+      <c r="N18" s="6">
+        <v>0</v>
+      </c>
+      <c r="O18" s="6">
+        <v>0</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>0</v>
+      </c>
+      <c r="R18" s="9">
+        <v>0</v>
+      </c>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="51">
+        <v>11</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0</v>
+      </c>
+      <c r="J19" s="6">
+        <v>0</v>
+      </c>
+      <c r="K19" s="6">
+        <v>0</v>
+      </c>
+      <c r="L19" s="6">
+        <v>0</v>
+      </c>
+      <c r="M19" s="6">
+        <v>0</v>
+      </c>
+      <c r="N19" s="6">
+        <v>0</v>
+      </c>
+      <c r="O19" s="6">
+        <v>0</v>
+      </c>
+      <c r="P19" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>0</v>
+      </c>
+      <c r="R19" s="9">
+        <v>0</v>
+      </c>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="51">
+        <v>12</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0</v>
+      </c>
+      <c r="J20" s="6">
+        <v>0</v>
+      </c>
+      <c r="K20" s="6">
+        <v>0</v>
+      </c>
+      <c r="L20" s="6">
+        <v>0</v>
+      </c>
+      <c r="M20" s="6">
+        <v>0</v>
+      </c>
+      <c r="N20" s="6">
+        <v>0</v>
+      </c>
+      <c r="O20" s="6">
+        <v>0</v>
+      </c>
+      <c r="P20" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>0</v>
+      </c>
+      <c r="R20" s="9">
+        <v>0</v>
+      </c>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="51">
+        <v>13</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6">
+        <v>1</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
+        <v>1</v>
+      </c>
+      <c r="N21" s="6">
+        <v>1</v>
+      </c>
+      <c r="O21" s="6">
+        <v>1</v>
+      </c>
+      <c r="P21" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>0</v>
+      </c>
+      <c r="R21" s="9">
+        <v>0</v>
+      </c>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="51">
+        <v>14</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0</v>
+      </c>
+      <c r="J22" s="6">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6">
+        <v>0</v>
+      </c>
+      <c r="L22" s="6">
+        <v>0</v>
+      </c>
+      <c r="M22" s="6">
+        <v>0</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0</v>
+      </c>
+      <c r="O22" s="6">
+        <v>0</v>
+      </c>
+      <c r="P22" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>0</v>
+      </c>
+      <c r="R22" s="9">
+        <v>0</v>
+      </c>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+    </row>
+    <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="52">
+        <v>15</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0</v>
+      </c>
+      <c r="G23" s="11">
+        <v>0</v>
+      </c>
+      <c r="H23" s="11">
+        <v>0</v>
+      </c>
+      <c r="I23" s="11">
+        <v>0</v>
+      </c>
+      <c r="J23" s="11">
+        <v>0</v>
+      </c>
+      <c r="K23" s="11">
+        <v>0</v>
+      </c>
+      <c r="L23" s="11">
+        <v>0</v>
+      </c>
+      <c r="M23" s="11">
+        <v>0</v>
+      </c>
+      <c r="N23" s="11">
+        <v>0</v>
+      </c>
+      <c r="O23" s="11">
+        <v>0</v>
+      </c>
+      <c r="P23" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="11">
+        <v>0</v>
+      </c>
+      <c r="R23" s="13">
+        <v>0</v>
+      </c>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="30"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edit `task-2` in `desicion-support`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/decision-support/task-2/task-2.xlsx
+++ b/3-course-6-semester/decision-support/task-2/task-2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\egor\github\university\3-course-6-semester\decision-support\task-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronn\Documents\github\university\3-course-6-semester\decision-support\task-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91462E76-BE17-4E9B-B372-FBBB535BD377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA8DDCF-2297-4302-BBB3-EC8562C4E95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{737F3F3F-B8D1-487C-8F75-3BB915F47FFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="5" xr2:uid="{737F3F3F-B8D1-487C-8F75-3BB915F47FFB}"/>
   </bookViews>
   <sheets>
     <sheet name="(Criteria) Данные" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="(Criteria) Тесты" sheetId="3" r:id="rId3"/>
     <sheet name="(Pareto) Данные" sheetId="4" r:id="rId4"/>
     <sheet name="(Pareto) Матрица" sheetId="5" r:id="rId5"/>
+    <sheet name="(Lexicographic opt) Прямой" sheetId="6" r:id="rId6"/>
+    <sheet name="(Lexicographic opt) Обратный" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="59">
   <si>
     <t>ВТБ</t>
   </si>
@@ -211,12 +213,18 @@
   <si>
     <t>max</t>
   </si>
+  <si>
+    <t>Приоритет</t>
+  </si>
+  <si>
+    <t>Ранг</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +263,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -288,7 +303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -584,11 +599,221 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -676,15 +901,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -712,6 +928,113 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1052,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A4A19C-CE63-4B26-AAA3-ADCE19EB590C}">
   <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
@@ -1078,7 +1401,7 @@
     </row>
     <row r="3" spans="2:14" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="30"/>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="50" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -1115,7 +1438,7 @@
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="30"/>
-      <c r="C4" s="42"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
@@ -1150,7 +1473,7 @@
     </row>
     <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="30"/>
-      <c r="C5" s="43"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="3">
         <v>11.5</v>
       </c>
@@ -1796,7 +2119,7 @@
     </row>
     <row r="3" spans="2:18" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="30"/>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="50" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -1836,7 +2159,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="30"/>
-      <c r="C4" s="42"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
@@ -1875,7 +2198,7 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="30"/>
-      <c r="C5" s="43"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="3">
         <v>11.5</v>
       </c>
@@ -3100,10 +3423,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47085B6B-A0C8-470C-BF16-E059821430EF}">
-  <dimension ref="B6:K24"/>
+  <dimension ref="B4:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="L26" sqref="B5:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3111,9 +3434,38 @@
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:11" ht="109.5" x14ac:dyDescent="0.25">
-      <c r="C7" s="41" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+    </row>
+    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+    </row>
+    <row r="7" spans="2:12" ht="109.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="30"/>
+      <c r="C7" s="50" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="21" t="s">
@@ -3140,9 +3492,11 @@
       <c r="K7" s="22" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="42"/>
+      <c r="L7" s="30"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="30"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
@@ -3167,9 +3521,11 @@
       <c r="K8" s="23" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="43"/>
+      <c r="L8" s="30"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="30"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="36" t="s">
         <v>55</v>
       </c>
@@ -3194,9 +3550,10 @@
       <c r="K9" s="37" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="L9" s="30"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="30">
         <v>1</v>
       </c>
       <c r="C10" s="25" t="s">
@@ -3226,9 +3583,10 @@
       <c r="K10" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="L10" s="30"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="30">
         <v>2</v>
       </c>
       <c r="C11" s="25" t="s">
@@ -3258,41 +3616,43 @@
       <c r="K11" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="L11" s="30"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="30">
         <v>3</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="53">
         <v>11.5</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="53">
         <v>10</v>
       </c>
-      <c r="F12" s="38">
-        <v>1</v>
-      </c>
-      <c r="G12" s="38">
+      <c r="F12" s="53">
+        <v>1</v>
+      </c>
+      <c r="G12" s="53">
         <v>5</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="53">
         <v>25</v>
       </c>
-      <c r="I12" s="38">
+      <c r="I12" s="53">
         <v>10.75</v>
       </c>
-      <c r="J12" s="38">
+      <c r="J12" s="53">
         <v>60</v>
       </c>
-      <c r="K12" s="40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="5">
+      <c r="K12" s="54">
+        <v>1</v>
+      </c>
+      <c r="L12" s="30"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="30">
         <v>4</v>
       </c>
       <c r="C13" s="25" t="s">
@@ -3322,9 +3682,10 @@
       <c r="K13" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
+      <c r="L13" s="30"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="30">
         <v>5</v>
       </c>
       <c r="C14" s="25" t="s">
@@ -3354,9 +3715,10 @@
       <c r="K14" s="40">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="5">
+      <c r="L14" s="30"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="30">
         <v>6</v>
       </c>
       <c r="C15" s="25" t="s">
@@ -3386,9 +3748,10 @@
       <c r="K15" s="40">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="5">
+      <c r="L15" s="30"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="30">
         <v>7</v>
       </c>
       <c r="C16" s="25" t="s">
@@ -3418,9 +3781,10 @@
       <c r="K16" s="40">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="5">
+      <c r="L16" s="30"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="30">
         <v>8</v>
       </c>
       <c r="C17" s="25" t="s">
@@ -3450,9 +3814,10 @@
       <c r="K17" s="40">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
+      <c r="L17" s="30"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="30">
         <v>9</v>
       </c>
       <c r="C18" s="25" t="s">
@@ -3482,9 +3847,10 @@
       <c r="K18" s="40">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="5">
+      <c r="L18" s="30"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="30">
         <v>10</v>
       </c>
       <c r="C19" s="25" t="s">
@@ -3514,9 +3880,10 @@
       <c r="K19" s="40">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
+      <c r="L19" s="30"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="30">
         <v>11</v>
       </c>
       <c r="C20" s="25" t="s">
@@ -3546,9 +3913,10 @@
       <c r="K20" s="40">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="5">
+      <c r="L20" s="30"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="30">
         <v>12</v>
       </c>
       <c r="C21" s="25" t="s">
@@ -3578,9 +3946,10 @@
       <c r="K21" s="40">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="5">
+      <c r="L21" s="30"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="30">
         <v>13</v>
       </c>
       <c r="C22" s="25" t="s">
@@ -3610,9 +3979,10 @@
       <c r="K22" s="40">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="5">
+      <c r="L22" s="30"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="30">
         <v>14</v>
       </c>
       <c r="C23" s="25" t="s">
@@ -3642,9 +4012,10 @@
       <c r="K23" s="40">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="5">
+      <c r="L23" s="30"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="30">
         <v>15</v>
       </c>
       <c r="C24" s="27" t="s">
@@ -3674,6 +4045,33 @@
       <c r="K24" s="29">
         <v>1.5</v>
       </c>
+      <c r="L24" s="30"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3687,8 +4085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F66624-DBED-43C6-BC18-B91A3DB8C019}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3854,49 +4252,49 @@
       <c r="A8" s="30"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
-      <c r="D8" s="47">
-        <v>1</v>
-      </c>
-      <c r="E8" s="48">
+      <c r="D8" s="44">
+        <v>1</v>
+      </c>
+      <c r="E8" s="45">
         <v>2</v>
       </c>
-      <c r="F8" s="48">
+      <c r="F8" s="45">
         <v>3</v>
       </c>
-      <c r="G8" s="48">
+      <c r="G8" s="45">
         <v>4</v>
       </c>
-      <c r="H8" s="48">
+      <c r="H8" s="45">
         <v>5</v>
       </c>
-      <c r="I8" s="48">
+      <c r="I8" s="45">
         <v>6</v>
       </c>
-      <c r="J8" s="48">
+      <c r="J8" s="45">
         <v>7</v>
       </c>
-      <c r="K8" s="48">
+      <c r="K8" s="45">
         <v>8</v>
       </c>
-      <c r="L8" s="48">
+      <c r="L8" s="45">
         <v>9</v>
       </c>
-      <c r="M8" s="48">
+      <c r="M8" s="45">
         <v>10</v>
       </c>
-      <c r="N8" s="48">
+      <c r="N8" s="45">
         <v>11</v>
       </c>
-      <c r="O8" s="48">
+      <c r="O8" s="45">
         <v>12</v>
       </c>
-      <c r="P8" s="48">
+      <c r="P8" s="45">
         <v>13</v>
       </c>
-      <c r="Q8" s="48">
+      <c r="Q8" s="45">
         <v>14</v>
       </c>
-      <c r="R8" s="49">
+      <c r="R8" s="46">
         <v>15</v>
       </c>
       <c r="S8" s="30"/>
@@ -3905,52 +4303,52 @@
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
-      <c r="C9" s="50">
-        <v>1</v>
-      </c>
-      <c r="D9" s="44">
-        <v>0</v>
-      </c>
-      <c r="E9" s="45">
-        <v>0</v>
-      </c>
-      <c r="F9" s="45">
-        <v>0</v>
-      </c>
-      <c r="G9" s="45">
-        <v>0</v>
-      </c>
-      <c r="H9" s="45">
-        <v>0</v>
-      </c>
-      <c r="I9" s="45">
-        <v>0</v>
-      </c>
-      <c r="J9" s="45">
-        <v>0</v>
-      </c>
-      <c r="K9" s="45">
-        <v>0</v>
-      </c>
-      <c r="L9" s="45">
-        <v>0</v>
-      </c>
-      <c r="M9" s="45">
-        <v>0</v>
-      </c>
-      <c r="N9" s="45">
-        <v>0</v>
-      </c>
-      <c r="O9" s="45">
-        <v>0</v>
-      </c>
-      <c r="P9" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="45">
-        <v>0</v>
-      </c>
-      <c r="R9" s="46">
+      <c r="C9" s="47">
+        <v>1</v>
+      </c>
+      <c r="D9" s="41">
+        <v>0</v>
+      </c>
+      <c r="E9" s="42">
+        <v>0</v>
+      </c>
+      <c r="F9" s="42">
+        <v>0</v>
+      </c>
+      <c r="G9" s="42">
+        <v>0</v>
+      </c>
+      <c r="H9" s="42">
+        <v>0</v>
+      </c>
+      <c r="I9" s="42">
+        <v>0</v>
+      </c>
+      <c r="J9" s="42">
+        <v>0</v>
+      </c>
+      <c r="K9" s="42">
+        <v>0</v>
+      </c>
+      <c r="L9" s="42">
+        <v>0</v>
+      </c>
+      <c r="M9" s="42">
+        <v>0</v>
+      </c>
+      <c r="N9" s="42">
+        <v>0</v>
+      </c>
+      <c r="O9" s="42">
+        <v>0</v>
+      </c>
+      <c r="P9" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="42">
+        <v>0</v>
+      </c>
+      <c r="R9" s="43">
         <v>0</v>
       </c>
       <c r="S9" s="30"/>
@@ -3959,7 +4357,7 @@
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
       <c r="B10" s="30"/>
-      <c r="C10" s="51">
+      <c r="C10" s="48">
         <v>2</v>
       </c>
       <c r="D10" s="8">
@@ -4013,7 +4411,7 @@
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
       <c r="B11" s="30"/>
-      <c r="C11" s="51">
+      <c r="C11" s="48">
         <v>3</v>
       </c>
       <c r="D11" s="8">
@@ -4067,7 +4465,7 @@
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
       <c r="B12" s="30"/>
-      <c r="C12" s="51">
+      <c r="C12" s="48">
         <v>4</v>
       </c>
       <c r="D12" s="8">
@@ -4121,7 +4519,7 @@
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
       <c r="B13" s="30"/>
-      <c r="C13" s="51">
+      <c r="C13" s="48">
         <v>5</v>
       </c>
       <c r="D13" s="8">
@@ -4175,7 +4573,7 @@
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" s="30"/>
-      <c r="C14" s="51">
+      <c r="C14" s="48">
         <v>6</v>
       </c>
       <c r="D14" s="8">
@@ -4229,7 +4627,7 @@
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
       <c r="B15" s="30"/>
-      <c r="C15" s="51">
+      <c r="C15" s="48">
         <v>7</v>
       </c>
       <c r="D15" s="8">
@@ -4283,7 +4681,7 @@
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
       <c r="B16" s="30"/>
-      <c r="C16" s="51">
+      <c r="C16" s="48">
         <v>8</v>
       </c>
       <c r="D16" s="8">
@@ -4337,7 +4735,7 @@
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
       <c r="B17" s="30"/>
-      <c r="C17" s="51">
+      <c r="C17" s="48">
         <v>9</v>
       </c>
       <c r="D17" s="8">
@@ -4391,7 +4789,7 @@
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
       <c r="B18" s="30"/>
-      <c r="C18" s="51">
+      <c r="C18" s="48">
         <v>10</v>
       </c>
       <c r="D18" s="8">
@@ -4445,7 +4843,7 @@
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="30"/>
-      <c r="C19" s="51">
+      <c r="C19" s="48">
         <v>11</v>
       </c>
       <c r="D19" s="8">
@@ -4499,7 +4897,7 @@
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
       <c r="B20" s="30"/>
-      <c r="C20" s="51">
+      <c r="C20" s="48">
         <v>12</v>
       </c>
       <c r="D20" s="8">
@@ -4553,7 +4951,7 @@
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
       <c r="B21" s="30"/>
-      <c r="C21" s="51">
+      <c r="C21" s="48">
         <v>13</v>
       </c>
       <c r="D21" s="8">
@@ -4607,7 +5005,7 @@
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
       <c r="B22" s="30"/>
-      <c r="C22" s="51">
+      <c r="C22" s="48">
         <v>14</v>
       </c>
       <c r="D22" s="8">
@@ -4661,7 +5059,7 @@
     <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
       <c r="B23" s="30"/>
-      <c r="C23" s="52">
+      <c r="C23" s="49">
         <v>15</v>
       </c>
       <c r="D23" s="10">
@@ -4845,4 +5243,2264 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC371177-2B82-43B9-8DFB-4DA6946502E7}">
+  <dimension ref="C6:V27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+    </row>
+    <row r="7" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="30"/>
+      <c r="D7" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="76">
+        <v>1</v>
+      </c>
+      <c r="F7" s="55"/>
+      <c r="G7" s="76">
+        <v>2</v>
+      </c>
+      <c r="H7" s="55"/>
+      <c r="I7" s="76">
+        <v>3</v>
+      </c>
+      <c r="J7" s="55"/>
+      <c r="K7" s="76">
+        <v>4</v>
+      </c>
+      <c r="L7" s="55"/>
+      <c r="M7" s="86">
+        <v>5</v>
+      </c>
+      <c r="N7" s="56"/>
+      <c r="O7" s="86">
+        <v>6</v>
+      </c>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="86">
+        <v>7</v>
+      </c>
+      <c r="R7" s="56"/>
+      <c r="S7" s="75">
+        <v>8</v>
+      </c>
+      <c r="T7" s="56"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+    </row>
+    <row r="8" spans="3:22" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="30"/>
+      <c r="D8" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="78"/>
+      <c r="G8" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="71"/>
+      <c r="I8" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="71"/>
+      <c r="K8" s="84" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="71"/>
+      <c r="M8" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="71"/>
+      <c r="O8" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="R8" s="72"/>
+      <c r="S8" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="T8" s="87"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="30"/>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C9" s="30"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="88"/>
+      <c r="T9" s="89"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C10" s="30"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="P10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="R10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="S10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="T10" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C11" s="30">
+        <v>1</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="66">
+        <v>13.2</v>
+      </c>
+      <c r="F11" s="81">
+        <v>10</v>
+      </c>
+      <c r="G11" s="83">
+        <v>0</v>
+      </c>
+      <c r="H11" s="81">
+        <v>12</v>
+      </c>
+      <c r="I11" s="83">
+        <v>1.3</v>
+      </c>
+      <c r="J11" s="81">
+        <v>14</v>
+      </c>
+      <c r="K11" s="83">
+        <v>14</v>
+      </c>
+      <c r="L11" s="81">
+        <v>14</v>
+      </c>
+      <c r="M11" s="66">
+        <v>25</v>
+      </c>
+      <c r="N11" s="81">
+        <v>14</v>
+      </c>
+      <c r="O11" s="66">
+        <v>11.45</v>
+      </c>
+      <c r="P11" s="81">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="83">
+        <v>65</v>
+      </c>
+      <c r="R11" s="81">
+        <v>14</v>
+      </c>
+      <c r="S11" s="83">
+        <v>1</v>
+      </c>
+      <c r="T11" s="26">
+        <v>14</v>
+      </c>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C12" s="30">
+        <v>2</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="66">
+        <v>14</v>
+      </c>
+      <c r="F12" s="81">
+        <v>11</v>
+      </c>
+      <c r="G12" s="66">
+        <v>10</v>
+      </c>
+      <c r="H12" s="81">
+        <v>13</v>
+      </c>
+      <c r="I12" s="66">
+        <v>1</v>
+      </c>
+      <c r="J12" s="81">
+        <v>15</v>
+      </c>
+      <c r="K12" s="66">
+        <v>5</v>
+      </c>
+      <c r="L12" s="81">
+        <v>15</v>
+      </c>
+      <c r="M12" s="66">
+        <v>37.5</v>
+      </c>
+      <c r="N12" s="81">
+        <v>15</v>
+      </c>
+      <c r="O12" s="83">
+        <v>12.45</v>
+      </c>
+      <c r="P12" s="81">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="83">
+        <v>65</v>
+      </c>
+      <c r="R12" s="81">
+        <v>15</v>
+      </c>
+      <c r="S12" s="83">
+        <v>1</v>
+      </c>
+      <c r="T12" s="26">
+        <v>15</v>
+      </c>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C13" s="30">
+        <v>3</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="67">
+        <v>11.5</v>
+      </c>
+      <c r="F13" s="90">
+        <v>4</v>
+      </c>
+      <c r="G13" s="91">
+        <v>10</v>
+      </c>
+      <c r="H13" s="90">
+        <v>6</v>
+      </c>
+      <c r="I13" s="67">
+        <v>1</v>
+      </c>
+      <c r="J13" s="81">
+        <v>8</v>
+      </c>
+      <c r="K13" s="67">
+        <v>5</v>
+      </c>
+      <c r="L13" s="81">
+        <v>8</v>
+      </c>
+      <c r="M13" s="67">
+        <v>25</v>
+      </c>
+      <c r="N13" s="81">
+        <v>8</v>
+      </c>
+      <c r="O13" s="67">
+        <v>10.75</v>
+      </c>
+      <c r="P13" s="81">
+        <v>8</v>
+      </c>
+      <c r="Q13" s="67">
+        <v>60</v>
+      </c>
+      <c r="R13" s="81">
+        <v>8</v>
+      </c>
+      <c r="S13" s="67">
+        <v>1</v>
+      </c>
+      <c r="T13" s="26">
+        <v>8</v>
+      </c>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C14" s="30">
+        <v>4</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="66">
+        <v>12.5</v>
+      </c>
+      <c r="F14" s="81">
+        <v>8</v>
+      </c>
+      <c r="G14" s="66">
+        <v>10</v>
+      </c>
+      <c r="H14" s="81">
+        <v>10</v>
+      </c>
+      <c r="I14" s="66">
+        <v>1.2</v>
+      </c>
+      <c r="J14" s="81">
+        <v>12</v>
+      </c>
+      <c r="K14" s="66">
+        <v>4</v>
+      </c>
+      <c r="L14" s="81">
+        <v>12</v>
+      </c>
+      <c r="M14" s="83">
+        <v>12.5</v>
+      </c>
+      <c r="N14" s="81">
+        <v>12</v>
+      </c>
+      <c r="O14" s="83">
+        <v>11.6</v>
+      </c>
+      <c r="P14" s="81">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="83">
+        <v>65</v>
+      </c>
+      <c r="R14" s="81">
+        <v>12</v>
+      </c>
+      <c r="S14" s="83">
+        <v>1</v>
+      </c>
+      <c r="T14" s="26">
+        <v>12</v>
+      </c>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C15" s="30">
+        <v>5</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="66">
+        <v>12</v>
+      </c>
+      <c r="F15" s="93">
+        <v>7</v>
+      </c>
+      <c r="G15" s="66">
+        <v>10</v>
+      </c>
+      <c r="H15" s="81">
+        <v>9</v>
+      </c>
+      <c r="I15" s="66">
+        <v>0</v>
+      </c>
+      <c r="J15" s="81">
+        <v>11</v>
+      </c>
+      <c r="K15" s="66">
+        <v>18</v>
+      </c>
+      <c r="L15" s="81">
+        <v>11</v>
+      </c>
+      <c r="M15" s="66">
+        <v>25</v>
+      </c>
+      <c r="N15" s="81">
+        <v>11</v>
+      </c>
+      <c r="O15" s="66">
+        <v>10.75</v>
+      </c>
+      <c r="P15" s="81">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="66">
+        <v>75</v>
+      </c>
+      <c r="R15" s="81">
+        <v>11</v>
+      </c>
+      <c r="S15" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="T15" s="26">
+        <v>11</v>
+      </c>
+      <c r="U15" s="30"/>
+      <c r="V15" s="30"/>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C16" s="30">
+        <v>6</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="66">
+        <v>7.05</v>
+      </c>
+      <c r="F16" s="81">
+        <v>1</v>
+      </c>
+      <c r="G16" s="66">
+        <v>5</v>
+      </c>
+      <c r="H16" s="81">
+        <v>1</v>
+      </c>
+      <c r="I16" s="66">
+        <v>1</v>
+      </c>
+      <c r="J16" s="81">
+        <v>1</v>
+      </c>
+      <c r="K16" s="66">
+        <v>1</v>
+      </c>
+      <c r="L16" s="81">
+        <v>1</v>
+      </c>
+      <c r="M16" s="66">
+        <v>37.5</v>
+      </c>
+      <c r="N16" s="81">
+        <v>1</v>
+      </c>
+      <c r="O16" s="66">
+        <v>5.5250000000000004</v>
+      </c>
+      <c r="P16" s="81">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="66">
+        <v>69</v>
+      </c>
+      <c r="R16" s="81">
+        <v>1</v>
+      </c>
+      <c r="S16" s="66">
+        <v>2</v>
+      </c>
+      <c r="T16" s="26">
+        <v>1</v>
+      </c>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C17" s="30">
+        <v>7</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="66">
+        <v>11</v>
+      </c>
+      <c r="F17" s="81">
+        <v>3</v>
+      </c>
+      <c r="G17" s="66">
+        <v>15</v>
+      </c>
+      <c r="H17" s="81">
+        <v>4</v>
+      </c>
+      <c r="I17" s="66">
+        <v>1</v>
+      </c>
+      <c r="J17" s="81">
+        <v>4</v>
+      </c>
+      <c r="K17" s="66">
+        <v>3</v>
+      </c>
+      <c r="L17" s="81">
+        <v>4</v>
+      </c>
+      <c r="M17" s="66">
+        <v>7.5</v>
+      </c>
+      <c r="N17" s="81">
+        <v>4</v>
+      </c>
+      <c r="O17" s="66">
+        <v>9.5</v>
+      </c>
+      <c r="P17" s="81">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="66">
+        <v>55</v>
+      </c>
+      <c r="R17" s="81">
+        <v>4</v>
+      </c>
+      <c r="S17" s="66">
+        <v>1</v>
+      </c>
+      <c r="T17" s="26">
+        <v>4</v>
+      </c>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C18" s="30">
+        <v>8</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="66">
+        <v>13</v>
+      </c>
+      <c r="F18" s="81">
+        <v>9</v>
+      </c>
+      <c r="G18" s="66">
+        <v>0</v>
+      </c>
+      <c r="H18" s="81">
+        <v>11</v>
+      </c>
+      <c r="I18" s="66">
+        <v>1</v>
+      </c>
+      <c r="J18" s="81">
+        <v>13</v>
+      </c>
+      <c r="K18" s="66">
+        <v>5</v>
+      </c>
+      <c r="L18" s="81">
+        <v>13</v>
+      </c>
+      <c r="M18" s="66">
+        <v>25</v>
+      </c>
+      <c r="N18" s="81">
+        <v>13</v>
+      </c>
+      <c r="O18" s="66">
+        <v>11</v>
+      </c>
+      <c r="P18" s="81">
+        <v>13</v>
+      </c>
+      <c r="Q18" s="66">
+        <v>60</v>
+      </c>
+      <c r="R18" s="81">
+        <v>13</v>
+      </c>
+      <c r="S18" s="66">
+        <v>2</v>
+      </c>
+      <c r="T18" s="26">
+        <v>13</v>
+      </c>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C19" s="30">
+        <v>9</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="66">
+        <v>11</v>
+      </c>
+      <c r="F19" s="81">
+        <v>3</v>
+      </c>
+      <c r="G19" s="66">
+        <v>30</v>
+      </c>
+      <c r="H19" s="81">
+        <v>3</v>
+      </c>
+      <c r="I19" s="66">
+        <v>0</v>
+      </c>
+      <c r="J19" s="81">
+        <v>3</v>
+      </c>
+      <c r="K19" s="66">
+        <v>1</v>
+      </c>
+      <c r="L19" s="81">
+        <v>3</v>
+      </c>
+      <c r="M19" s="66">
+        <v>7.5</v>
+      </c>
+      <c r="N19" s="81">
+        <v>3</v>
+      </c>
+      <c r="O19" s="66">
+        <v>10</v>
+      </c>
+      <c r="P19" s="81">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="66">
+        <v>70</v>
+      </c>
+      <c r="R19" s="81">
+        <v>3</v>
+      </c>
+      <c r="S19" s="66">
+        <v>1</v>
+      </c>
+      <c r="T19" s="26">
+        <v>3</v>
+      </c>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C20" s="30">
+        <v>10</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="66">
+        <v>11.5</v>
+      </c>
+      <c r="F20" s="90">
+        <v>4</v>
+      </c>
+      <c r="G20" s="92">
+        <v>15</v>
+      </c>
+      <c r="H20" s="93">
+        <v>5</v>
+      </c>
+      <c r="I20" s="66">
+        <v>1</v>
+      </c>
+      <c r="J20" s="81">
+        <v>6</v>
+      </c>
+      <c r="K20" s="66">
+        <v>5</v>
+      </c>
+      <c r="L20" s="81">
+        <v>6</v>
+      </c>
+      <c r="M20" s="66">
+        <v>12.5</v>
+      </c>
+      <c r="N20" s="81">
+        <v>6</v>
+      </c>
+      <c r="O20" s="66">
+        <v>10.25</v>
+      </c>
+      <c r="P20" s="81">
+        <v>6</v>
+      </c>
+      <c r="Q20" s="66">
+        <v>60</v>
+      </c>
+      <c r="R20" s="81">
+        <v>6</v>
+      </c>
+      <c r="S20" s="66">
+        <v>0.25</v>
+      </c>
+      <c r="T20" s="26">
+        <v>6</v>
+      </c>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C21" s="30">
+        <v>11</v>
+      </c>
+      <c r="D21" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="66">
+        <v>11.8</v>
+      </c>
+      <c r="F21" s="93">
+        <v>5</v>
+      </c>
+      <c r="G21" s="66">
+        <v>10</v>
+      </c>
+      <c r="H21" s="81">
+        <v>7</v>
+      </c>
+      <c r="I21" s="66">
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="81">
+        <v>9</v>
+      </c>
+      <c r="K21" s="66">
+        <v>5</v>
+      </c>
+      <c r="L21" s="81">
+        <v>9</v>
+      </c>
+      <c r="M21" s="66">
+        <v>50</v>
+      </c>
+      <c r="N21" s="81">
+        <v>9</v>
+      </c>
+      <c r="O21" s="66">
+        <v>10.65</v>
+      </c>
+      <c r="P21" s="81">
+        <v>9</v>
+      </c>
+      <c r="Q21" s="66">
+        <v>70</v>
+      </c>
+      <c r="R21" s="81">
+        <v>9</v>
+      </c>
+      <c r="S21" s="66">
+        <v>2</v>
+      </c>
+      <c r="T21" s="26">
+        <v>9</v>
+      </c>
+      <c r="U21" s="30"/>
+      <c r="V21" s="30"/>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C22" s="30">
+        <v>12</v>
+      </c>
+      <c r="D22" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="66">
+        <v>11.9</v>
+      </c>
+      <c r="F22" s="93">
+        <v>6</v>
+      </c>
+      <c r="G22" s="66">
+        <v>15</v>
+      </c>
+      <c r="H22" s="81">
+        <v>8</v>
+      </c>
+      <c r="I22" s="66">
+        <v>1.5</v>
+      </c>
+      <c r="J22" s="81">
+        <v>10</v>
+      </c>
+      <c r="K22" s="66">
+        <v>7</v>
+      </c>
+      <c r="L22" s="81">
+        <v>10</v>
+      </c>
+      <c r="M22" s="66">
+        <v>37.5</v>
+      </c>
+      <c r="N22" s="81">
+        <v>10</v>
+      </c>
+      <c r="O22" s="66">
+        <v>10.45</v>
+      </c>
+      <c r="P22" s="81">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="66">
+        <v>60</v>
+      </c>
+      <c r="R22" s="81">
+        <v>10</v>
+      </c>
+      <c r="S22" s="66">
+        <v>2</v>
+      </c>
+      <c r="T22" s="26">
+        <v>10</v>
+      </c>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C23" s="30">
+        <v>13</v>
+      </c>
+      <c r="D23" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="66">
+        <v>11.5</v>
+      </c>
+      <c r="F23" s="90">
+        <v>4</v>
+      </c>
+      <c r="G23" s="92">
+        <v>15</v>
+      </c>
+      <c r="H23" s="93">
+        <v>5</v>
+      </c>
+      <c r="I23" s="66">
+        <v>0.8</v>
+      </c>
+      <c r="J23" s="81">
+        <v>5</v>
+      </c>
+      <c r="K23" s="66">
+        <v>3</v>
+      </c>
+      <c r="L23" s="81">
+        <v>5</v>
+      </c>
+      <c r="M23" s="66">
+        <v>50</v>
+      </c>
+      <c r="N23" s="81">
+        <v>5</v>
+      </c>
+      <c r="O23" s="66">
+        <v>10.25</v>
+      </c>
+      <c r="P23" s="81">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="66">
+        <v>54</v>
+      </c>
+      <c r="R23" s="81">
+        <v>5</v>
+      </c>
+      <c r="S23" s="66">
+        <v>1</v>
+      </c>
+      <c r="T23" s="26">
+        <v>5</v>
+      </c>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C24" s="30">
+        <v>14</v>
+      </c>
+      <c r="D24" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="66">
+        <v>11.5</v>
+      </c>
+      <c r="F24" s="90">
+        <v>4</v>
+      </c>
+      <c r="G24" s="92">
+        <v>10</v>
+      </c>
+      <c r="H24" s="90">
+        <v>6</v>
+      </c>
+      <c r="I24" s="66">
+        <v>0</v>
+      </c>
+      <c r="J24" s="81">
+        <v>7</v>
+      </c>
+      <c r="K24" s="66">
+        <v>5</v>
+      </c>
+      <c r="L24" s="81">
+        <v>7</v>
+      </c>
+      <c r="M24" s="66">
+        <v>12.5</v>
+      </c>
+      <c r="N24" s="81">
+        <v>7</v>
+      </c>
+      <c r="O24" s="66">
+        <v>10.5</v>
+      </c>
+      <c r="P24" s="81">
+        <v>7</v>
+      </c>
+      <c r="Q24" s="66">
+        <v>60</v>
+      </c>
+      <c r="R24" s="81">
+        <v>7</v>
+      </c>
+      <c r="S24" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="T24" s="26">
+        <v>7</v>
+      </c>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+    </row>
+    <row r="25" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="30">
+        <v>15</v>
+      </c>
+      <c r="D25" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="68">
+        <v>10.5</v>
+      </c>
+      <c r="F25" s="82">
+        <v>2</v>
+      </c>
+      <c r="G25" s="68">
+        <v>25</v>
+      </c>
+      <c r="H25" s="82">
+        <v>2</v>
+      </c>
+      <c r="I25" s="85">
+        <v>3</v>
+      </c>
+      <c r="J25" s="82">
+        <v>2</v>
+      </c>
+      <c r="K25" s="85">
+        <v>5</v>
+      </c>
+      <c r="L25" s="82">
+        <v>2</v>
+      </c>
+      <c r="M25" s="85">
+        <v>7.5</v>
+      </c>
+      <c r="N25" s="82">
+        <v>2</v>
+      </c>
+      <c r="O25" s="85">
+        <v>9.625</v>
+      </c>
+      <c r="P25" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="85">
+        <v>60</v>
+      </c>
+      <c r="R25" s="82">
+        <v>2</v>
+      </c>
+      <c r="S25" s="85">
+        <v>1.5</v>
+      </c>
+      <c r="T25" s="29">
+        <v>2</v>
+      </c>
+      <c r="U25" s="30"/>
+      <c r="V25" s="30"/>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="30"/>
+    </row>
+    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="Q8:R9"/>
+    <mergeCell ref="S8:T9"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="G8:H9"/>
+    <mergeCell ref="I8:J9"/>
+    <mergeCell ref="K8:L9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="O8:P9"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A51BEF0-27CE-49CD-85E7-39CE3BDA5D0A}">
+  <dimension ref="C6:V27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+    </row>
+    <row r="7" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="30"/>
+      <c r="D7" s="94" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="75">
+        <v>1</v>
+      </c>
+      <c r="F7" s="56"/>
+      <c r="G7" s="86">
+        <v>2</v>
+      </c>
+      <c r="H7" s="56"/>
+      <c r="I7" s="86">
+        <v>3</v>
+      </c>
+      <c r="J7" s="56"/>
+      <c r="K7" s="86">
+        <v>4</v>
+      </c>
+      <c r="L7" s="56"/>
+      <c r="M7" s="76">
+        <v>5</v>
+      </c>
+      <c r="N7" s="55"/>
+      <c r="O7" s="76">
+        <v>6</v>
+      </c>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="76">
+        <v>7</v>
+      </c>
+      <c r="R7" s="55"/>
+      <c r="S7" s="76">
+        <v>8</v>
+      </c>
+      <c r="T7" s="77"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+    </row>
+    <row r="8" spans="3:22" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="30"/>
+      <c r="D8" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="87"/>
+      <c r="G8" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="72"/>
+      <c r="I8" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="78"/>
+      <c r="K8" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="71"/>
+      <c r="M8" s="84" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="71"/>
+      <c r="O8" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="71"/>
+      <c r="S8" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="T8" s="62"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="30"/>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C9" s="30"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="79"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="64"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C10" s="30"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="P10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q10" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="S10" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="T10" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C11" s="30">
+        <v>1</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="83">
+        <v>1</v>
+      </c>
+      <c r="F11" s="40">
+        <v>3</v>
+      </c>
+      <c r="G11" s="83">
+        <v>65</v>
+      </c>
+      <c r="H11" s="93">
+        <v>7</v>
+      </c>
+      <c r="I11" s="66">
+        <v>11.45</v>
+      </c>
+      <c r="J11" s="81">
+        <v>7</v>
+      </c>
+      <c r="K11" s="66">
+        <v>25</v>
+      </c>
+      <c r="L11" s="81">
+        <v>7</v>
+      </c>
+      <c r="M11" s="83">
+        <v>14</v>
+      </c>
+      <c r="N11" s="81">
+        <v>7</v>
+      </c>
+      <c r="O11" s="83">
+        <v>1.3</v>
+      </c>
+      <c r="P11" s="81">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="83">
+        <v>0</v>
+      </c>
+      <c r="R11" s="81">
+        <v>7</v>
+      </c>
+      <c r="S11" s="66">
+        <v>13.2</v>
+      </c>
+      <c r="T11" s="26">
+        <v>7</v>
+      </c>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C12" s="30">
+        <v>2</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="83">
+        <v>1</v>
+      </c>
+      <c r="F12" s="40">
+        <v>3</v>
+      </c>
+      <c r="G12" s="83">
+        <v>65</v>
+      </c>
+      <c r="H12" s="93">
+        <v>7</v>
+      </c>
+      <c r="I12" s="83">
+        <v>12.45</v>
+      </c>
+      <c r="J12" s="81">
+        <v>9</v>
+      </c>
+      <c r="K12" s="66">
+        <v>37.5</v>
+      </c>
+      <c r="L12" s="81">
+        <v>9</v>
+      </c>
+      <c r="M12" s="66">
+        <v>5</v>
+      </c>
+      <c r="N12" s="81">
+        <v>9</v>
+      </c>
+      <c r="O12" s="66">
+        <v>1</v>
+      </c>
+      <c r="P12" s="81">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="66">
+        <v>10</v>
+      </c>
+      <c r="R12" s="81">
+        <v>9</v>
+      </c>
+      <c r="S12" s="66">
+        <v>14</v>
+      </c>
+      <c r="T12" s="26">
+        <v>9</v>
+      </c>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C13" s="30">
+        <v>3</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="67">
+        <v>1</v>
+      </c>
+      <c r="F13" s="40">
+        <v>3</v>
+      </c>
+      <c r="G13" s="67">
+        <v>60</v>
+      </c>
+      <c r="H13" s="81">
+        <v>6</v>
+      </c>
+      <c r="I13" s="67">
+        <v>10.75</v>
+      </c>
+      <c r="J13" s="81">
+        <v>6</v>
+      </c>
+      <c r="K13" s="67">
+        <v>25</v>
+      </c>
+      <c r="L13" s="81">
+        <v>6</v>
+      </c>
+      <c r="M13" s="67">
+        <v>5</v>
+      </c>
+      <c r="N13" s="81">
+        <v>6</v>
+      </c>
+      <c r="O13" s="67">
+        <v>1</v>
+      </c>
+      <c r="P13" s="81">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="91">
+        <v>10</v>
+      </c>
+      <c r="R13" s="81">
+        <v>6</v>
+      </c>
+      <c r="S13" s="67">
+        <v>11.5</v>
+      </c>
+      <c r="T13" s="26">
+        <v>6</v>
+      </c>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C14" s="30">
+        <v>4</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="83">
+        <v>1</v>
+      </c>
+      <c r="F14" s="40">
+        <v>3</v>
+      </c>
+      <c r="G14" s="83">
+        <v>65</v>
+      </c>
+      <c r="H14" s="93">
+        <v>7</v>
+      </c>
+      <c r="I14" s="83">
+        <v>11.6</v>
+      </c>
+      <c r="J14" s="81">
+        <v>8</v>
+      </c>
+      <c r="K14" s="83">
+        <v>12.5</v>
+      </c>
+      <c r="L14" s="81">
+        <v>8</v>
+      </c>
+      <c r="M14" s="66">
+        <v>4</v>
+      </c>
+      <c r="N14" s="81">
+        <v>8</v>
+      </c>
+      <c r="O14" s="66">
+        <v>1.2</v>
+      </c>
+      <c r="P14" s="81">
+        <v>8</v>
+      </c>
+      <c r="Q14" s="66">
+        <v>10</v>
+      </c>
+      <c r="R14" s="81">
+        <v>8</v>
+      </c>
+      <c r="S14" s="66">
+        <v>12.5</v>
+      </c>
+      <c r="T14" s="26">
+        <v>8</v>
+      </c>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C15" s="30">
+        <v>5</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="40">
+        <v>2</v>
+      </c>
+      <c r="G15" s="66">
+        <v>75</v>
+      </c>
+      <c r="H15" s="81">
+        <v>3</v>
+      </c>
+      <c r="I15" s="66">
+        <v>10.75</v>
+      </c>
+      <c r="J15" s="81">
+        <v>3</v>
+      </c>
+      <c r="K15" s="66">
+        <v>25</v>
+      </c>
+      <c r="L15" s="81">
+        <v>3</v>
+      </c>
+      <c r="M15" s="66">
+        <v>18</v>
+      </c>
+      <c r="N15" s="81">
+        <v>3</v>
+      </c>
+      <c r="O15" s="66">
+        <v>0</v>
+      </c>
+      <c r="P15" s="81">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="66">
+        <v>10</v>
+      </c>
+      <c r="R15" s="81">
+        <v>3</v>
+      </c>
+      <c r="S15" s="66">
+        <v>12</v>
+      </c>
+      <c r="T15" s="26">
+        <v>3</v>
+      </c>
+      <c r="U15" s="30"/>
+      <c r="V15" s="30"/>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C16" s="30">
+        <v>6</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="66">
+        <v>2</v>
+      </c>
+      <c r="F16" s="40">
+        <v>5</v>
+      </c>
+      <c r="G16" s="66">
+        <v>69</v>
+      </c>
+      <c r="H16" s="81">
+        <v>11</v>
+      </c>
+      <c r="I16" s="66">
+        <v>5.5250000000000004</v>
+      </c>
+      <c r="J16" s="81">
+        <v>14</v>
+      </c>
+      <c r="K16" s="66">
+        <v>37.5</v>
+      </c>
+      <c r="L16" s="81">
+        <v>14</v>
+      </c>
+      <c r="M16" s="66">
+        <v>1</v>
+      </c>
+      <c r="N16" s="81">
+        <v>14</v>
+      </c>
+      <c r="O16" s="66">
+        <v>1</v>
+      </c>
+      <c r="P16" s="81">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="66">
+        <v>5</v>
+      </c>
+      <c r="R16" s="81">
+        <v>14</v>
+      </c>
+      <c r="S16" s="66">
+        <v>7.05</v>
+      </c>
+      <c r="T16" s="26">
+        <v>14</v>
+      </c>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C17" s="30">
+        <v>7</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="66">
+        <v>1</v>
+      </c>
+      <c r="F17" s="40">
+        <v>3</v>
+      </c>
+      <c r="G17" s="66">
+        <v>55</v>
+      </c>
+      <c r="H17" s="81">
+        <v>5</v>
+      </c>
+      <c r="I17" s="66">
+        <v>9.5</v>
+      </c>
+      <c r="J17" s="81">
+        <v>5</v>
+      </c>
+      <c r="K17" s="66">
+        <v>7.5</v>
+      </c>
+      <c r="L17" s="81">
+        <v>5</v>
+      </c>
+      <c r="M17" s="66">
+        <v>3</v>
+      </c>
+      <c r="N17" s="81">
+        <v>5</v>
+      </c>
+      <c r="O17" s="66">
+        <v>1</v>
+      </c>
+      <c r="P17" s="81">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="66">
+        <v>15</v>
+      </c>
+      <c r="R17" s="81">
+        <v>5</v>
+      </c>
+      <c r="S17" s="66">
+        <v>11</v>
+      </c>
+      <c r="T17" s="26">
+        <v>5</v>
+      </c>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C18" s="30">
+        <v>8</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="66">
+        <v>2</v>
+      </c>
+      <c r="F18" s="40">
+        <v>5</v>
+      </c>
+      <c r="G18" s="66">
+        <v>60</v>
+      </c>
+      <c r="H18" s="93">
+        <v>10</v>
+      </c>
+      <c r="I18" s="66">
+        <v>11</v>
+      </c>
+      <c r="J18" s="81">
+        <v>13</v>
+      </c>
+      <c r="K18" s="66">
+        <v>25</v>
+      </c>
+      <c r="L18" s="81">
+        <v>13</v>
+      </c>
+      <c r="M18" s="66">
+        <v>5</v>
+      </c>
+      <c r="N18" s="81">
+        <v>13</v>
+      </c>
+      <c r="O18" s="66">
+        <v>1</v>
+      </c>
+      <c r="P18" s="81">
+        <v>13</v>
+      </c>
+      <c r="Q18" s="66">
+        <v>0</v>
+      </c>
+      <c r="R18" s="81">
+        <v>13</v>
+      </c>
+      <c r="S18" s="66">
+        <v>13</v>
+      </c>
+      <c r="T18" s="26">
+        <v>13</v>
+      </c>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C19" s="30">
+        <v>9</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="66">
+        <v>1</v>
+      </c>
+      <c r="F19" s="40">
+        <v>3</v>
+      </c>
+      <c r="G19" s="66">
+        <v>70</v>
+      </c>
+      <c r="H19" s="93">
+        <v>8</v>
+      </c>
+      <c r="I19" s="66">
+        <v>10</v>
+      </c>
+      <c r="J19" s="81">
+        <v>10</v>
+      </c>
+      <c r="K19" s="66">
+        <v>7.5</v>
+      </c>
+      <c r="L19" s="81">
+        <v>10</v>
+      </c>
+      <c r="M19" s="66">
+        <v>1</v>
+      </c>
+      <c r="N19" s="81">
+        <v>10</v>
+      </c>
+      <c r="O19" s="66">
+        <v>0</v>
+      </c>
+      <c r="P19" s="81">
+        <v>10</v>
+      </c>
+      <c r="Q19" s="66">
+        <v>30</v>
+      </c>
+      <c r="R19" s="81">
+        <v>10</v>
+      </c>
+      <c r="S19" s="66">
+        <v>11</v>
+      </c>
+      <c r="T19" s="26">
+        <v>10</v>
+      </c>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C20" s="30">
+        <v>10</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="66">
+        <v>0.25</v>
+      </c>
+      <c r="F20" s="40">
+        <v>1</v>
+      </c>
+      <c r="G20" s="66">
+        <v>60</v>
+      </c>
+      <c r="H20" s="93">
+        <v>1</v>
+      </c>
+      <c r="I20" s="66">
+        <v>10.25</v>
+      </c>
+      <c r="J20" s="81">
+        <v>1</v>
+      </c>
+      <c r="K20" s="66">
+        <v>12.5</v>
+      </c>
+      <c r="L20" s="81">
+        <v>1</v>
+      </c>
+      <c r="M20" s="66">
+        <v>5</v>
+      </c>
+      <c r="N20" s="81">
+        <v>1</v>
+      </c>
+      <c r="O20" s="66">
+        <v>1</v>
+      </c>
+      <c r="P20" s="81">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="92">
+        <v>15</v>
+      </c>
+      <c r="R20" s="81">
+        <v>1</v>
+      </c>
+      <c r="S20" s="66">
+        <v>11.5</v>
+      </c>
+      <c r="T20" s="26">
+        <v>1</v>
+      </c>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C21" s="30">
+        <v>11</v>
+      </c>
+      <c r="D21" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="66">
+        <v>2</v>
+      </c>
+      <c r="F21" s="40">
+        <v>5</v>
+      </c>
+      <c r="G21" s="66">
+        <v>70</v>
+      </c>
+      <c r="H21" s="93">
+        <v>12</v>
+      </c>
+      <c r="I21" s="66">
+        <v>10.65</v>
+      </c>
+      <c r="J21" s="81">
+        <v>15</v>
+      </c>
+      <c r="K21" s="66">
+        <v>50</v>
+      </c>
+      <c r="L21" s="81">
+        <v>15</v>
+      </c>
+      <c r="M21" s="66">
+        <v>5</v>
+      </c>
+      <c r="N21" s="81">
+        <v>15</v>
+      </c>
+      <c r="O21" s="66">
+        <v>0.8</v>
+      </c>
+      <c r="P21" s="81">
+        <v>15</v>
+      </c>
+      <c r="Q21" s="66">
+        <v>10</v>
+      </c>
+      <c r="R21" s="81">
+        <v>15</v>
+      </c>
+      <c r="S21" s="66">
+        <v>11.8</v>
+      </c>
+      <c r="T21" s="26">
+        <v>15</v>
+      </c>
+      <c r="U21" s="30"/>
+      <c r="V21" s="30"/>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C22" s="30">
+        <v>12</v>
+      </c>
+      <c r="D22" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="66">
+        <v>2</v>
+      </c>
+      <c r="F22" s="40">
+        <v>5</v>
+      </c>
+      <c r="G22" s="66">
+        <v>60</v>
+      </c>
+      <c r="H22" s="93">
+        <v>10</v>
+      </c>
+      <c r="I22" s="66">
+        <v>10.45</v>
+      </c>
+      <c r="J22" s="81">
+        <v>12</v>
+      </c>
+      <c r="K22" s="66">
+        <v>37.5</v>
+      </c>
+      <c r="L22" s="81">
+        <v>12</v>
+      </c>
+      <c r="M22" s="66">
+        <v>7</v>
+      </c>
+      <c r="N22" s="81">
+        <v>12</v>
+      </c>
+      <c r="O22" s="66">
+        <v>1.5</v>
+      </c>
+      <c r="P22" s="81">
+        <v>12</v>
+      </c>
+      <c r="Q22" s="66">
+        <v>15</v>
+      </c>
+      <c r="R22" s="81">
+        <v>12</v>
+      </c>
+      <c r="S22" s="66">
+        <v>11.9</v>
+      </c>
+      <c r="T22" s="26">
+        <v>12</v>
+      </c>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C23" s="30">
+        <v>13</v>
+      </c>
+      <c r="D23" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="66">
+        <v>1</v>
+      </c>
+      <c r="F23" s="40">
+        <v>3</v>
+      </c>
+      <c r="G23" s="66">
+        <v>54</v>
+      </c>
+      <c r="H23" s="81">
+        <v>4</v>
+      </c>
+      <c r="I23" s="66">
+        <v>10.25</v>
+      </c>
+      <c r="J23" s="81">
+        <v>4</v>
+      </c>
+      <c r="K23" s="66">
+        <v>50</v>
+      </c>
+      <c r="L23" s="81">
+        <v>4</v>
+      </c>
+      <c r="M23" s="66">
+        <v>3</v>
+      </c>
+      <c r="N23" s="81">
+        <v>4</v>
+      </c>
+      <c r="O23" s="66">
+        <v>0.8</v>
+      </c>
+      <c r="P23" s="81">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="92">
+        <v>15</v>
+      </c>
+      <c r="R23" s="81">
+        <v>4</v>
+      </c>
+      <c r="S23" s="66">
+        <v>11.5</v>
+      </c>
+      <c r="T23" s="26">
+        <v>4</v>
+      </c>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C24" s="30">
+        <v>14</v>
+      </c>
+      <c r="D24" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="40">
+        <v>2</v>
+      </c>
+      <c r="G24" s="66">
+        <v>60</v>
+      </c>
+      <c r="H24" s="81">
+        <v>2</v>
+      </c>
+      <c r="I24" s="66">
+        <v>10.5</v>
+      </c>
+      <c r="J24" s="81">
+        <v>2</v>
+      </c>
+      <c r="K24" s="66">
+        <v>12.5</v>
+      </c>
+      <c r="L24" s="81">
+        <v>2</v>
+      </c>
+      <c r="M24" s="66">
+        <v>5</v>
+      </c>
+      <c r="N24" s="81">
+        <v>2</v>
+      </c>
+      <c r="O24" s="66">
+        <v>0</v>
+      </c>
+      <c r="P24" s="81">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="92">
+        <v>10</v>
+      </c>
+      <c r="R24" s="81">
+        <v>2</v>
+      </c>
+      <c r="S24" s="66">
+        <v>11.5</v>
+      </c>
+      <c r="T24" s="26">
+        <v>2</v>
+      </c>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+    </row>
+    <row r="25" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="30">
+        <v>15</v>
+      </c>
+      <c r="D25" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="85">
+        <v>1.5</v>
+      </c>
+      <c r="F25" s="95">
+        <v>4</v>
+      </c>
+      <c r="G25" s="85">
+        <v>60</v>
+      </c>
+      <c r="H25" s="96">
+        <v>9</v>
+      </c>
+      <c r="I25" s="85">
+        <v>9.625</v>
+      </c>
+      <c r="J25" s="82">
+        <v>11</v>
+      </c>
+      <c r="K25" s="85">
+        <v>7.5</v>
+      </c>
+      <c r="L25" s="82">
+        <v>11</v>
+      </c>
+      <c r="M25" s="85">
+        <v>5</v>
+      </c>
+      <c r="N25" s="82">
+        <v>11</v>
+      </c>
+      <c r="O25" s="85">
+        <v>3</v>
+      </c>
+      <c r="P25" s="82">
+        <v>11</v>
+      </c>
+      <c r="Q25" s="68">
+        <v>25</v>
+      </c>
+      <c r="R25" s="82">
+        <v>11</v>
+      </c>
+      <c r="S25" s="68">
+        <v>10.5</v>
+      </c>
+      <c r="T25" s="29">
+        <v>11</v>
+      </c>
+      <c r="U25" s="30"/>
+      <c r="V25" s="30"/>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="30"/>
+    </row>
+    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="S8:T9"/>
+    <mergeCell ref="Q8:R9"/>
+    <mergeCell ref="O8:P9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="K8:L9"/>
+    <mergeCell ref="I8:J9"/>
+    <mergeCell ref="G8:H9"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="I7:J7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>